<commit_message>
amelioration visuel dans les resultat
</commit_message>
<xml_diff>
--- a/SKU_(V2.1) BOM unifié électrique-mécanique.xlsx
+++ b/SKU_(V2.1) BOM unifié électrique-mécanique.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://noovelia-my.sharepoint.com/personal/vcasaubon_noovelia_com/Documents/Documents/GitHub/SKU-Generetor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_094AAEE62D4C983F153B3595395BDA1626CB13DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B6F2727-58EA-41E7-BE93-1E706087F481}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_2C0B0735BDC20D4C66F543A87058EFF2F7CAD29A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F383348-F163-4C10-A366-644BBBB9C7D9}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKU_Électrique" sheetId="1" r:id="rId1"/>
@@ -5455,8 +5455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10643,8 +10643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H279"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="B265" sqref="B265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Améliore la génération et le format des SKU industriels
Refonte du README avec documentation détaillée sur le format SKU, installation et cas d'usage. Ajout d'un alphabet industriel sécurisé, d'un mapping de types étendu et d'une logique d'optimisation pour éviter les redondances dans les SKU. Ajout de la conversion de séquence en base industrielle, de tests unitaires pour la génération optimisée et la normalisation, et d'un script de comparaison des formats SKU. Mise à jour des dépendances dans requirements.txt.
</commit_message>
<xml_diff>
--- a/SKU_(V2.1) BOM unifié électrique-mécanique.xlsx
+++ b/SKU_(V2.1) BOM unifié électrique-mécanique.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://noovelia-my.sharepoint.com/personal/vcasaubon_noovelia_com/Documents/Documents/GitHub/SKU-Generetor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcasaubon.NOOVELIA\OneDrive - Noovelia\Documents\GitHub\SKU-Generetor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_2C0B0735BDC20D4C66F543A87058EFF2F7CAD29A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F383348-F163-4C10-A366-644BBBB9C7D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60218C7A-5EC4-48D2-AE3C-AFD92C922F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>Domain</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-CCSS-00001</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAA</t>
   </si>
   <si>
     <t>D-ST 2,5</t>
@@ -74,7 +74,7 @@
     <t>ÉLECTRIQUE</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-CCSS-00002</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAB</t>
   </si>
   <si>
     <t>D-ST 2,5-QUATTRO</t>
@@ -89,7 +89,7 @@
     <t>TBCV1, TBCV2, TBCV3, TBCV4, TBCV5, TBCV6, TBCV7, TBCV11, TBCV12, TBCV13, TBCV14, TBCV15, TBCV16</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-DPTT-00001</t>
+    <t>ELEC-ELEC-STD-DPTTRS-AAAA</t>
   </si>
   <si>
     <t>EBC116</t>
@@ -107,7 +107,7 @@
     <t>SPL1, SPL2, SPL3</t>
   </si>
   <si>
-    <t>ELEC-POWER-STD-LMNT-00001</t>
+    <t>ELEC-POWER-STD-LMNTTO-AAAA</t>
   </si>
   <si>
     <t>DSM155Q030W075PB</t>
@@ -125,7 +125,7 @@
     <t>C1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RRTS-00001</t>
+    <t>ELEC-ELEC-STD-RRTSDR-AAAA</t>
   </si>
   <si>
     <t>XB7NS8444</t>
@@ -143,7 +143,7 @@
     <t>S5, S6, S7, S8, S9, S10</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00001</t>
+    <t>ELEC-ASS-STD-MONTER-AAAA</t>
   </si>
   <si>
     <t>1072F12-05-2-1-S-00050</t>
@@ -161,7 +161,7 @@
     <t>WH6, WH80</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00002</t>
+    <t>ELEC-ASS-STD-MONTER-AAAB</t>
   </si>
   <si>
     <t>1406102</t>
@@ -173,7 +173,7 @@
     <t>WH5</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00003</t>
+    <t>ELEC-ASS-STD-MONTER-AAAC</t>
   </si>
   <si>
     <t>1408742</t>
@@ -185,7 +185,7 @@
     <t>WH9</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00004</t>
+    <t>ELEC-ASS-STD-MONTER-AAAD</t>
   </si>
   <si>
     <t>21349292405030</t>
@@ -200,7 +200,7 @@
     <t>WH16</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00005</t>
+    <t>ELEC-ASS-STD-MONTER-AAAE</t>
   </si>
   <si>
     <t>EC0711</t>
@@ -212,7 +212,7 @@
     <t>WH7</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00006</t>
+    <t>ELEC-ASS-STD-MONTER-AAAF</t>
   </si>
   <si>
     <t>GRIP-RGB-C1-10-12</t>
@@ -227,7 +227,7 @@
     <t>WH21, WH22, WH23, WH24, WH33</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00007</t>
+    <t>ELEC-ASS-STD-MONTER-AAAG</t>
   </si>
   <si>
     <t>GRIP-RGB-C1-10-36</t>
@@ -239,7 +239,7 @@
     <t>WH20</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00008</t>
+    <t>ELEC-ASS-STD-MONTER-AAAH</t>
   </si>
   <si>
     <t>M12A05FL-12AFL-SB001</t>
@@ -254,7 +254,7 @@
     <t>WH40</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00009</t>
+    <t>ELEC-ASS-STD-MONTER-AAAJ</t>
   </si>
   <si>
     <t>M12A08MR-12AMR-SBA05</t>
@@ -266,7 +266,7 @@
     <t>WH1, WH4</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00010</t>
+    <t>ELEC-ASS-STD-MONTER-AAAK</t>
   </si>
   <si>
     <t>MSAS-05BFFM-SL8J02</t>
@@ -278,7 +278,7 @@
     <t>WH39</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00011</t>
+    <t>ELEC-ASS-STD-MONTER-AAAM</t>
   </si>
   <si>
     <t>NANSX-AAACAEZZ1</t>
@@ -293,7 +293,7 @@
     <t>WH12, WH17</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00012</t>
+    <t>ELEC-ASS-STD-MONTER-AAAN</t>
   </si>
   <si>
     <t>P582-003</t>
@@ -308,7 +308,7 @@
     <t>WH36</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00013</t>
+    <t>ELEC-ASS-STD-MONTER-AAAP</t>
   </si>
   <si>
     <t>SC-3AAK003F</t>
@@ -323,7 +323,7 @@
     <t>WH37</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00014</t>
+    <t>ELEC-ASS-STD-MONTER-AAAQ</t>
   </si>
   <si>
     <t>T4061310004-001</t>
@@ -338,7 +338,7 @@
     <t>WH14, WH19</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00015</t>
+    <t>ELEC-ASS-STD-MONTER-AAAR</t>
   </si>
   <si>
     <t>T4161320005-002</t>
@@ -350,7 +350,7 @@
     <t>WH13, WH18, WH38, WH42</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00016</t>
+    <t>ELEC-ASS-STD-MONTER-AAAS</t>
   </si>
   <si>
     <t>TAA751A5501-002</t>
@@ -362,7 +362,7 @@
     <t>WH81</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00017</t>
+    <t>ELEC-ASS-STD-MONTER-AAAT</t>
   </si>
   <si>
     <t>TAD14541111-020</t>
@@ -374,7 +374,7 @@
     <t>WH41</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00018</t>
+    <t>ELEC-ASS-STD-MONTER-AAAW</t>
   </si>
   <si>
     <t>TAD14741111-001</t>
@@ -386,7 +386,7 @@
     <t>WH8</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00019</t>
+    <t>ELEC-ASS-STD-MONTER-AAAX</t>
   </si>
   <si>
     <t>TAD14741111-002</t>
@@ -398,7 +398,7 @@
     <t>WH11</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00020</t>
+    <t>ELEC-ASS-STD-MONTER-AAAY</t>
   </si>
   <si>
     <t>TCD14741111-001</t>
@@ -410,7 +410,7 @@
     <t>WH43, WH44</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00021</t>
+    <t>ELEC-ASS-STD-MONTER-AAAZ</t>
   </si>
   <si>
     <t>YF2A2D-020UV2XLEAX</t>
@@ -425,7 +425,7 @@
     <t>WH10</t>
   </si>
   <si>
-    <t>ELEC-ASS-ASM-SSMB-00022</t>
+    <t>ELEC-ASS-STD-MONTER-AAA2</t>
   </si>
   <si>
     <t>YF2A2D-050UV2XLEAX</t>
@@ -440,7 +440,7 @@
     <t>WH15</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-TMTS-00001</t>
+    <t>ELEC-ELEC-STD-TOMTSA-AAAA</t>
   </si>
   <si>
     <t>CR711S</t>
@@ -455,7 +455,7 @@
     <t>PLC1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-AUTR-00001</t>
+    <t>ELEC-ELEC-STD-AUTRE-AAAA</t>
   </si>
   <si>
     <t>90330</t>
@@ -473,7 +473,7 @@
     <t>MEC8</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRTS-00001</t>
+    <t>ELEC-ELEC-STD-VRTSSR-AAAA</t>
   </si>
   <si>
     <t>56525T42</t>
@@ -491,7 +491,7 @@
     <t>BZ1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-BTTR-00001</t>
+    <t>ELEC-ELEC-STD-BTTRSA-AAAA</t>
   </si>
   <si>
     <t>M-48V60-TRX</t>
@@ -515,7 +515,7 @@
     <t>BAT1, BAT2, BAT3, (BAT4 selon le client)</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00001</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAA</t>
   </si>
   <si>
     <t>10127815-08LF</t>
@@ -530,7 +530,7 @@
     <t>J1, J3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00002</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAB</t>
   </si>
   <si>
     <t>1321-BK</t>
@@ -545,7 +545,7 @@
     <t>P11, P15, P18, P22</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00003</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAC</t>
   </si>
   <si>
     <t>1321G1-BK</t>
@@ -557,7 +557,7 @@
     <t>P10, P14, P17, P21, P42</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00004</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAD</t>
   </si>
   <si>
     <t>1321G3-BK</t>
@@ -569,7 +569,7 @@
     <t>P9, P13, P16, P20, P43</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00005</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAE</t>
   </si>
   <si>
     <t>1381G1-BK</t>
@@ -581,7 +581,7 @@
     <t>P5, P8</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00006</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAF</t>
   </si>
   <si>
     <t>1381G3-BK</t>
@@ -593,7 +593,7 @@
     <t>P6, P7</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00007</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAG</t>
   </si>
   <si>
     <t>5916G4-BK</t>
@@ -605,7 +605,7 @@
     <t>P1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00008</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAH</t>
   </si>
   <si>
     <t>5916G5-BK</t>
@@ -617,7 +617,7 @@
     <t>P3, P4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00009</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAJ</t>
   </si>
   <si>
     <t>5916G7-BK</t>
@@ -629,7 +629,7 @@
     <t>P2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00010</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAK</t>
   </si>
   <si>
     <t>776164-1</t>
@@ -641,7 +641,7 @@
     <t>X1, X2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00011</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAM</t>
   </si>
   <si>
     <t>DT04-08PA-L012</t>
@@ -653,7 +653,7 @@
     <t>P35</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00012</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAN</t>
   </si>
   <si>
     <t>DT04-08PB-L012</t>
@@ -665,7 +665,7 @@
     <t>P34, P36</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00013</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAP</t>
   </si>
   <si>
     <t>DT04-12PA-BL04</t>
@@ -677,7 +677,7 @@
     <t>P37</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00014</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAQ</t>
   </si>
   <si>
     <t>DT04-12PB-L012</t>
@@ -689,7 +689,7 @@
     <t>P12, P19, P32</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00015</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAR</t>
   </si>
   <si>
     <t>DT04-2P</t>
@@ -701,7 +701,7 @@
     <t>P26, P27, P28, P29, P31</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00016</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAS</t>
   </si>
   <si>
     <t>DT04-4P-L012</t>
@@ -713,7 +713,7 @@
     <t>P33</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00017</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAT</t>
   </si>
   <si>
     <t>DT04-6P</t>
@@ -725,7 +725,7 @@
     <t>P24, P25, P30</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00018</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAW</t>
   </si>
   <si>
     <t>DT06-12SA</t>
@@ -737,7 +737,7 @@
     <t>J2, J4, J6, J18</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00019</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAX</t>
   </si>
   <si>
     <t>DT06-12SB</t>
@@ -749,7 +749,7 @@
     <t>J5</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00020</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAY</t>
   </si>
   <si>
     <t>DT06-2S</t>
@@ -761,7 +761,7 @@
     <t>J9, J10, J11, J12, J14</t>
   </si>
   <si>
-    <t>ELEC-ELEC-ENCL-BTRS-00021</t>
+    <t>ELEC-ELEC-ENCL-BOITIE-AAAZ</t>
   </si>
   <si>
     <t>DT06-6S</t>
@@ -773,7 +773,7 @@
     <t>J7, J8, J13</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-BRNR-00001</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAC</t>
   </si>
   <si>
     <t>5073180</t>
@@ -791,7 +791,7 @@
     <t>TB1, TB4</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-BRNR-00002</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAD</t>
   </si>
   <si>
     <t>5075160</t>
@@ -803,7 +803,7 @@
     <t>TB2, TB3</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-BRNR-00003</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAE</t>
   </si>
   <si>
     <t>PT 2,5</t>
@@ -818,7 +818,7 @@
     <t>TB14.1, TB14.2, TB73, TB74</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-BRNR-00004</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAF</t>
   </si>
   <si>
     <t>PT 2,5 OR</t>
@@ -833,7 +833,7 @@
     <t>TB58, TB59, TB60, TB61, TB62, TB63, TB64, TB65, TB66, TB67, TB70, TB71</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-BRNR-00005</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAG</t>
   </si>
   <si>
     <t>PT 2,5-QUATTRO</t>
@@ -848,7 +848,7 @@
     <t>TB10.1, TB10.2, TB11.1, TB11.2, TB11.4, TB11.5, TB11.6, TB13, TB68, TB69, TB80, TB81, TB82, TB83, TB84, TB85, TB86, TB116.1, TB116.2, TB117.1, TB117.2, TB118.1, TB118.2, TB119, TB128</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-BRNR-00006</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAH</t>
   </si>
   <si>
     <t>PT 2,5-QUATTRO OR</t>
@@ -863,7 +863,7 @@
     <t>TB50, TB51, TB52, TB53, TB54, TB55, TB56, TB57</t>
   </si>
   <si>
-    <t>ELEC-TERM-STD-BRNR-00007</t>
+    <t>ELEC-TERM-STD-BORNIE-AAAJ</t>
   </si>
   <si>
     <t>PT 2,5-QUATTRO PE</t>
@@ -878,7 +878,7 @@
     <t>TB105.1, TB105.2, TB105.3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-BTNS-00001</t>
+    <t>ELEC-ELEC-STD-BOTONS-AAAA</t>
   </si>
   <si>
     <t>XB7NA33</t>
@@ -893,7 +893,7 @@
     <t>S3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-BTNS-00002</t>
+    <t>ELEC-ELEC-STD-BOTONS-AAAB</t>
   </si>
   <si>
     <t>XB7NA42</t>
@@ -905,7 +905,7 @@
     <t>S2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00001</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAA</t>
   </si>
   <si>
     <t>0460-202-16141</t>
@@ -920,7 +920,7 @@
     <t>CNT58, CNT79, CNT80, CNT81, CNT82, CNT83, CNT84, CNT91, CNT92, CNT93, CNT94, CNT95, CNT96, CNT99, CNT100, CNT105, CNT106, CNT107, CNT108, CNT111, CNT112, CNT113, CNT115, CNT151, CNT152, CNT153, CNT154, CNT155, CNT156, CNT161, CNT162, CNT163, CNT164, CNT165, CNT166, CNT167, CNT168, CNT169, CNT170, CNT171, CNT172, CNT173, CNT174, CNT175, CNT176, CNT177, CNT178, CNT179, CNT180, CNT181, CNT182, CNT183, CNT184, CNT185, CNT186, CNT187, CNT188, CNT189, CNT190, CNT191, CNT192, CNT193, CNT194, CNT195, CNT196, CNT197, CNT198, CNT199, CNT200, CNT201, CNT202, CNT203, CNT204, CNT205</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00002</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAB</t>
   </si>
   <si>
     <t>0460-202-20141</t>
@@ -932,7 +932,7 @@
     <t>PIN8, PIN9, PIN10, PIN11, PIN12, PIN13, PIN14, PIN15, PIN16, PIN17, PIN18, PIN19, PIN39, PIN40, PIN41, PIN42, PIN43, PIN44, PIN45, PIN46, PIN47, PIN48, PIN49, PIN50</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00003</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAC</t>
   </si>
   <si>
     <t>0462-201-16141</t>
@@ -944,7 +944,7 @@
     <t>CNT52, CNT53, CNT54, CNT55, CNT56, CNT57, CNT59, CNT60, CNT61, CNT62, CNT63, CNT64, CNT65, CNT66, CNT67, CNT68, CNT69, CNT70, CNT71, CNT72, CNT73, CNT74, CNT75, CNT76, CNT77, CNT78, CNT85, CNT86, CNT87, CNT88, CNT89, CNT90, CNT97, CNT98, CNT101, CNT102, CNT103, CNT104, CNT109, CNT110, CNT114, CNT116, CNT145, CNT146, CNT147, CNT148, CNT149, CNT150, CNT206, CNT207, CNT208, CNT209, CNT210, CNT211, CNT214</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00004</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAD</t>
   </si>
   <si>
     <t>0462-209-16141</t>
@@ -956,7 +956,7 @@
     <t>PIN74</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00005</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAE</t>
   </si>
   <si>
     <t>10127817-221LF</t>
@@ -968,7 +968,7 @@
     <t>PIN1, PIN2, PIN3, PIN4, PIN5, PIN6, PIN7, PIN32, PIN33, PIN34, PIN35, PIN36, PIN37, PIN38</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00006</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAF</t>
   </si>
   <si>
     <t>1307-BK</t>
@@ -980,7 +980,7 @@
     <t>CNT5, CNT6</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00007</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAG</t>
   </si>
   <si>
     <t>1319G4-BK</t>
@@ -992,7 +992,7 @@
     <t>CNT212, CNT213</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00008</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAH</t>
   </si>
   <si>
     <t>1319G6-BK</t>
@@ -1004,7 +1004,7 @@
     <t>CNT24, CNT25, CNT26, CNT27, CNT28, CNT29, CNT43, CNT44, CNT45, CNT46, CNT47, CNT48</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00009</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAJ</t>
   </si>
   <si>
     <t>1383-BK</t>
@@ -1016,7 +1016,7 @@
     <t>CNT7, CNT8, CNT9, CNT10</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00010</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAK</t>
   </si>
   <si>
     <t>5913-BK</t>
@@ -1028,7 +1028,7 @@
     <t>CNT1, CNT2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00011</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAM</t>
   </si>
   <si>
     <t>5953-BK</t>
@@ -1040,7 +1040,7 @@
     <t>CNT3, CNT4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00012</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAN</t>
   </si>
   <si>
     <t>770854-1</t>
@@ -1052,7 +1052,7 @@
     <t>CNT11, CNT12, CNT13, CNT14, CNT15, CNT16, CNT17, CNT18, CNT19, CNT20, CNT21, CNT22, CNT23, CNT30, CNT31, CNT32, CNT33, CNT34, CNT35, CNT36, CNT37, CNT38, CNT39, CNT40, CNT41, CNT42</t>
   </si>
   <si>
-    <t>ELEC-ELEC-PIN-BRCH-00013</t>
+    <t>ELEC-ELEC-PIN-BROCHE-AAAP</t>
   </si>
   <si>
     <t>84-2480</t>
@@ -1067,7 +1067,7 @@
     <t>PIN20, PIN21, PIN22, PIN23, PIN24, PIN25, PIN26, PIN27, PIN28, PIN29, PIN30, PIN31, PIN51, PIN52, PIN53, PIN54, PIN55, PIN56, PIN57, PIN58, PIN59, PIN60, PIN61, PIN62</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CHRG-00001</t>
+    <t>ELEC-ELEC-STD-CHRGRS-AAAA</t>
   </si>
   <si>
     <t>100986</t>
@@ -1085,7 +1085,7 @@
     <t>CHG1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CHRG-00002</t>
+    <t>ELEC-ELEC-STD-CHRGRS-AAAB</t>
   </si>
   <si>
     <t>100993</t>
@@ -1097,7 +1097,7 @@
     <t>CHG2</t>
   </si>
   <si>
-    <t>ELEC-COMM-STD-CMMN-00001</t>
+    <t>ELEC-STD-STD-COMMNC-AAAA</t>
   </si>
   <si>
     <t>AL3050</t>
@@ -1115,7 +1115,7 @@
     <t>COM3</t>
   </si>
   <si>
-    <t>ELEC-COMM-STD-CMMN-00002</t>
+    <t>ELEC-STD-STD-COMMNC-AAAB</t>
   </si>
   <si>
     <t>ANT-DB1-WRT-RPS</t>
@@ -1130,7 +1130,7 @@
     <t>ANT1, ANT2</t>
   </si>
   <si>
-    <t>ELEC-COMM-STD-CMMN-00003</t>
+    <t>ELEC-STD-STD-COMMNC-AAAC</t>
   </si>
   <si>
     <t>AWK-1137C-US</t>
@@ -1145,7 +1145,7 @@
     <t>COM4</t>
   </si>
   <si>
-    <t>ELEC-COMM-STD-CMMN-00004</t>
+    <t>ELEC-STD-STD-COMMNC-AAAD</t>
   </si>
   <si>
     <t>CAN-ISO-2500-LVCUT</t>
@@ -1163,7 +1163,7 @@
     <t>COM5</t>
   </si>
   <si>
-    <t>ELEC-COMM-STD-CMMN-00005</t>
+    <t>ELEC-STD-STD-COMMNC-AAAE</t>
   </si>
   <si>
     <t>DTC510</t>
@@ -1175,7 +1175,7 @@
     <t>COM1, COM2</t>
   </si>
   <si>
-    <t>ELEC-CONN-STD-CNNC-00001</t>
+    <t>ELEC-STD-STD-CONNEC-AAAA</t>
   </si>
   <si>
     <t>221-412</t>
@@ -1193,7 +1193,7 @@
     <t>JP3, JP4, JP7, JP8, JP10</t>
   </si>
   <si>
-    <t>ELEC-CONN-STD-CNNC-00002</t>
+    <t>ELEC-STD-STD-CONNEC-AAAB</t>
   </si>
   <si>
     <t>4130</t>
@@ -1208,7 +1208,7 @@
     <t>J17</t>
   </si>
   <si>
-    <t>ELEC-CONN-STD-CNNC-00003</t>
+    <t>ELEC-STD-STD-CONNEC-AAAC</t>
   </si>
   <si>
     <t>50-00962</t>
@@ -1223,7 +1223,7 @@
     <t>P23</t>
   </si>
   <si>
-    <t>ELEC-CONN-STD-CNNC-00004</t>
+    <t>ELEC-STD-STD-CONNEC-AAAD</t>
   </si>
   <si>
     <t>AC-HDMI-RR</t>
@@ -1235,7 +1235,7 @@
     <t>J15</t>
   </si>
   <si>
-    <t>ELEC-CONN-STD-CNNC-00005</t>
+    <t>ELEC-STD-STD-CONNEC-AAAE</t>
   </si>
   <si>
     <t>AC-USB3-AAB</t>
@@ -1247,7 +1247,7 @@
     <t>J16</t>
   </si>
   <si>
-    <t>ELEC-CONN-STD-CNNC-00006</t>
+    <t>ELEC-STD-STD-CONNEC-AAAF</t>
   </si>
   <si>
     <t>T4111012051-000</t>
@@ -1259,7 +1259,7 @@
     <t>P38, P39, P40, P41, P44, P45</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00001</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAA</t>
   </si>
   <si>
     <t>PAC425T1-09C</t>
@@ -1280,7 +1280,7 @@
     <t>VFD1, VFD2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00002</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAB</t>
   </si>
   <si>
     <t>155124RS73200</t>
@@ -1298,7 +1298,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00003</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAC</t>
   </si>
   <si>
     <t>155124VS73200</t>
@@ -1310,7 +1310,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00004</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAD</t>
   </si>
   <si>
     <t>‎B077GTQV6K</t>
@@ -1325,7 +1325,7 @@
     <t>J1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00005</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAE</t>
   </si>
   <si>
     <t>RC1206FR-0710KL</t>
@@ -1340,7 +1340,7 @@
     <t>R1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00006</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAF</t>
   </si>
   <si>
     <t>1K6 1% 1206(3216)</t>
@@ -1355,7 +1355,7 @@
     <t>R2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00007</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAG</t>
   </si>
   <si>
     <t>RMCF1210JT3K60</t>
@@ -1370,7 +1370,7 @@
     <t>R3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00008</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAH</t>
   </si>
   <si>
     <t>RNCP1206FTD200R</t>
@@ -1382,7 +1382,7 @@
     <t>R4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00009</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAJ</t>
   </si>
   <si>
     <t>16591</t>
@@ -1397,7 +1397,7 @@
     <t>U1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00010</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAK</t>
   </si>
   <si>
     <t>Arduino Pro Micro</t>
@@ -1415,7 +1415,7 @@
     <t>U2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00011</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAM</t>
   </si>
   <si>
     <t>ASDS-ZH108</t>
@@ -1430,7 +1430,7 @@
     <t>U3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNTR-00012</t>
+    <t>ELEC-ELEC-STD-CONTRO-AAAN</t>
   </si>
   <si>
     <t>D-0055339</t>
@@ -1445,7 +1445,7 @@
     <t>Noovelia</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNVR-00001</t>
+    <t>ELEC-ELEC-STD-CONVRT-AAAA</t>
   </si>
   <si>
     <t>DDR-120C-24</t>
@@ -1463,7 +1463,7 @@
     <t>G3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNVR-00002</t>
+    <t>ELEC-ELEC-STD-CONVRT-AAAB</t>
   </si>
   <si>
     <t>DDR-240C-48</t>
@@ -1475,7 +1475,7 @@
     <t>G2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-CNVR-00003</t>
+    <t>ELEC-ELEC-STD-CONVRT-AAAC</t>
   </si>
   <si>
     <t>DDR-480C-24</t>
@@ -1487,7 +1487,7 @@
     <t>G1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00001</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAA</t>
   </si>
   <si>
     <t>0190020001</t>
@@ -1505,7 +1505,7 @@
     <t>CR43, CR109</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00002</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAB</t>
   </si>
   <si>
     <t>09130077Z</t>
@@ -1520,7 +1520,7 @@
     <t>CNT49, CNT50, CNT51</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00003</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAC</t>
   </si>
   <si>
     <t>160300</t>
@@ -1532,7 +1532,7 @@
     <t>CR28</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00004</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAD</t>
   </si>
   <si>
     <t>31811</t>
@@ -1544,7 +1544,7 @@
     <t>CR32</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00005</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAE</t>
   </si>
   <si>
     <t>33461</t>
@@ -1556,7 +1556,7 @@
     <t>CR33, CR35, CR36</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00006</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAF</t>
   </si>
   <si>
     <t>33463</t>
@@ -1568,7 +1568,7 @@
     <t>CR27</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00007</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAG</t>
   </si>
   <si>
     <t>33469</t>
@@ -1577,7 +1577,7 @@
     <t>CR31</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00008</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAH</t>
   </si>
   <si>
     <t>33471</t>
@@ -1589,7 +1589,7 @@
     <t>CR25, CR29</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00009</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAJ</t>
   </si>
   <si>
     <t>35772</t>
@@ -1601,7 +1601,7 @@
     <t>CR34</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00010</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAK</t>
   </si>
   <si>
     <t>913-053</t>
@@ -1613,7 +1613,7 @@
     <t>CR78, CR79, CR80, CR81, CR82, CR83, CR84, CR85</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00011</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAM</t>
   </si>
   <si>
     <t>913-058</t>
@@ -1625,7 +1625,7 @@
     <t>CR71, CR72, CR76, CR77, CR86, CR87, CR88, CR89, CR91, CR92, CR94, CR95, CR96, CR97, CR98, CR99, CR100, CR101, CR102, CR106, CR107, CR111</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00012</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAN</t>
   </si>
   <si>
     <t>913-059</t>
@@ -1637,7 +1637,7 @@
     <t>CR73, CR74, CR75, CR90, CR103, CR108</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00013</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAP</t>
   </si>
   <si>
     <t>A2-38R-C</t>
@@ -1652,7 +1652,7 @@
     <t>CR8, CR9, CR10, CR11, CR15, CR16, CR18, CR19, CR21, CR23, CR26</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00014</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAQ</t>
   </si>
   <si>
     <t>A2-56R-C</t>
@@ -1664,7 +1664,7 @@
     <t>CR1, CR2, CR3, CR4, CR5, CR37, CR38, CR40</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00015</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAR</t>
   </si>
   <si>
     <t>A6-56R-C</t>
@@ -1676,7 +1676,7 @@
     <t>CR41, CR42, CR52, CR53, CR55, CR56, CR57, CR58, CR59, CR60, CR61, CR62, CR63, CR64, CR65, CR66, CR67, CR68, CR69, CR70</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00016</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAS</t>
   </si>
   <si>
     <t>AI-50040N</t>
@@ -1691,7 +1691,7 @@
     <t>CR93</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00017</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAT</t>
   </si>
   <si>
     <t>AI-50042N</t>
@@ -1703,7 +1703,7 @@
     <t>CR39, CR47, CR110</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00018</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAW</t>
   </si>
   <si>
     <t>AI-50043N</t>
@@ -1715,7 +1715,7 @@
     <t>CR20, CR22</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00019</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAX</t>
   </si>
   <si>
     <t>AI-50100N</t>
@@ -1727,7 +1727,7 @@
     <t>CR105, CR112, CR113</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00020</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAY</t>
   </si>
   <si>
     <t>AI-50102N</t>
@@ -1739,7 +1739,7 @@
     <t>CR46, CR51, CR54, CR104</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00021</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAAZ</t>
   </si>
   <si>
     <t>AI-50209</t>
@@ -1751,7 +1751,7 @@
     <t>CR44, CR45</t>
   </si>
   <si>
-    <t>ELEC-ELEC-TERM-CSSS-00022</t>
+    <t>ELEC-ELEC-TERM-COSSES-AAA2</t>
   </si>
   <si>
     <t>LCA1-56F-E</t>
@@ -1763,7 +1763,7 @@
     <t>CR24, CR30, CR48, CR49, CR50</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-DIOD-00001</t>
+    <t>ELEC-ELEC-STD-DIODES-AAAA</t>
   </si>
   <si>
     <t>15SQ100</t>
@@ -1781,7 +1781,7 @@
     <t>D1, D2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-MBSS-00001</t>
+    <t>ELEC-ELEC-STD-MBSSEA-AAAA</t>
   </si>
   <si>
     <t>03540536Z</t>
@@ -1796,7 +1796,7 @@
     <t>KB2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-NCDR-00001</t>
+    <t>ELEC-ELEC-STD-NCODRS-AAAA</t>
   </si>
   <si>
     <t>TRN42-SRA4096R4096S4KN106</t>
@@ -1814,7 +1814,7 @@
     <t>ENC1, ENC2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-WIRE-FILX-00001</t>
+    <t>ELEC-ELEC-WIRE-FILAGE-AAAA</t>
   </si>
   <si>
     <t>Fil générique</t>
@@ -1832,7 +1832,7 @@
     <t>W1.1, W1.10, W1.11, W1.12, W1.13, W1.14, W1.15, W1.2, W1.3, W1.5, W1.6, W1.7, W1.8, W1.9, W2.1, W2.2, W2.3, W3.1, W4.1, W4.2, W4.3, W4.4, W4.5, W4.6, W4.7, W5.1, W6.1, W7.1, W8.1, W9.1, W9.2, W10.1, W10.2, W10.3, W10.4, W10.9, W11.1, W11.10, W11.11, W11.12, W11.13, W11.14, W11.15, W11.16, W11.6, W11.8, W11.9, W12.1, W13.1, W13.2, W13.3, W13.4, W14.1, W14.2, W15.1, W16.1, W18.1, W19.1, W20.1, W21.1, W22.1, W24.1, W25.1, W26.1, W27.1, W28.1, W28.2, W29.1, W30.1, W32.1, W33.1, W34.1, W35.1, W36.1, W37.1, W38.1, W39.1, W40.1, W41.1, W41.2, W42.1, W43.1, W44.1, W45.1, W46.1, W47.1, W48.1, W49.1, W50.1, W51.1, W52.1, W53.1, W54.1, W55.1, W56.1, W57.1, W58.1, W59.1, W60.1, W61.1, W62.1, W63.1, W64.1, W65.1, W66.1, W67.1, W68.1, W69.1, W70.1, W76.1, W77.1, W78.1, W79.1, W80.1, W82.1, W83.1, W84.1, W85.1, W86.1, W87.1, W88.1, W89.1, W90.1, W91.1, W93.1, W95.1, W96.1, W97.1, W98.1, W99.1, W100.1, W101.1, W102.1, W103.1, W104.1, W105.1, W107.1, W108.1, W109.1, W110.1, W111.1, W112.1, W113.1, W114.1, W115.1, W116.1, W117.1, W118.1, W120.1, W121.1, W122.1, W123.1, W124.1, W125.1, W128.1, W128.2, W129.1, W130.1, W130.2, W131.1, W132.1, W133.1, W134.1, W135.1, W136.1, W137.1, W138.1, W139.1, W140.1, W141.1, W142.1, W143.1, W144.1, W145.1, W146.1, W147.1, W148.1, W149.1, W150.1, W151.1, W156.1, W157.1, W162.1, W163.1, W168.1, W169.1, W170.1, W171.1, W176.1, W177.1, W182.1, W183.1, W184.1, W185.1, W194.1, W195.1, W196.1, W197.1, W198.1, W199.1, W200.1, W201.1, W202.1, W203.1, W205.1, W206.1, W207.1, W208.1, W208.2, W209.1, W209.2, W210.1, W211.1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00001</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAA</t>
   </si>
   <si>
     <t>142.5631.5302</t>
@@ -1847,7 +1847,7 @@
     <t>F4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00002</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAB</t>
   </si>
   <si>
     <t>142.5631.5702</t>
@@ -1859,7 +1859,7 @@
     <t>F2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00003</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAC</t>
   </si>
   <si>
     <t>142.5631.6102</t>
@@ -1871,7 +1871,7 @@
     <t>F3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00004</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAD</t>
   </si>
   <si>
     <t>166.7000.4502</t>
@@ -1883,7 +1883,7 @@
     <t>F29, F33, F34</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00005</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAE</t>
   </si>
   <si>
     <t>166.7000.5102</t>
@@ -1895,7 +1895,7 @@
     <t>F28</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00006</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAF</t>
   </si>
   <si>
     <t>166.7000.5152</t>
@@ -1907,7 +1907,7 @@
     <t>F30</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00007</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAG</t>
   </si>
   <si>
     <t>166.7000.5302</t>
@@ -1919,7 +1919,7 @@
     <t>F31, F32</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00008</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAH</t>
   </si>
   <si>
     <t>9005805.80</t>
@@ -1934,7 +1934,7 @@
     <t>F5, F6</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00009</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAJ</t>
   </si>
   <si>
     <t>ATC-1</t>
@@ -1949,7 +1949,7 @@
     <t>F12, F13, F14, F15, F19, F20, F21, F22, F23, F24, F25</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00010</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAK</t>
   </si>
   <si>
     <t>ATC-10</t>
@@ -1961,7 +1961,7 @@
     <t>F9, F10, F11</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00011</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAM</t>
   </si>
   <si>
     <t>ATC-2</t>
@@ -1973,7 +1973,7 @@
     <t>F7, F8, F16, F17, F27</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00012</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAN</t>
   </si>
   <si>
     <t>ATC-7.5</t>
@@ -1988,7 +1988,7 @@
     <t>F18, F26</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-FSBL-00013</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAP</t>
   </si>
   <si>
     <t>CNN250DIN</t>
@@ -2003,7 +2003,7 @@
     <t>F1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-GAIN-00001</t>
+    <t>ELEC-ELEC-STD-GAINES-AAAA</t>
   </si>
   <si>
     <t>CPA100-0750-BK</t>
@@ -2021,7 +2021,7 @@
     <t>HS1, HS2, HS3, HS4, HS5, HS19, HS20, HS24, HS25, HS29, HS31, HS33, HS34, HS40, HS42, HS44, HS45, HS46, HS47, HS48, HS49, HS50, HS51, HS52, HS53, HS54, HS55</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-GAIN-00002</t>
+    <t>ELEC-ELEC-STD-GAINES-AAAB</t>
   </si>
   <si>
     <t>CPA100-0750-RD</t>
@@ -2033,7 +2033,7 @@
     <t>HS8, HS9, HS10, HS11, HS12, HS16, HS18, HS21, HS22, HS23, HS26, HS27, HS28, HS30, HS32, HS35, HS36, HS37, HS38, HS39, HS41, HS43</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-LIDA-00001</t>
+    <t>ELEC-ELEC-STD-LIDAR-AAAA</t>
   </si>
   <si>
     <t>NANS3-CAAZ30AN1</t>
@@ -2051,7 +2051,7 @@
     <t>B2, B4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-LMRS-00001</t>
+    <t>ELEC-ELEC-STD-LMRSUI-AAAA</t>
   </si>
   <si>
     <t>NMS1217</t>
@@ -2072,7 +2072,7 @@
     <t>EC1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-MGNT-00001</t>
+    <t>ELEC-ELEC-STD-MGNTQS-AAAA</t>
   </si>
   <si>
     <t>MLSE-0300A2NP0</t>
@@ -2087,7 +2087,7 @@
     <t>B1, B3</t>
   </si>
   <si>
-    <t>ELEC-MOTOR-STD-MTRS-00001</t>
+    <t>ELEC-MOTOR-STD-MOTRSE-AAAA</t>
   </si>
   <si>
     <t>WD-L1C-900KG-261NM-43-1.2KW/34V/AC/IP44-EMB48VDC/M-ENC-READY</t>
@@ -2105,7 +2105,7 @@
     <t>M1, M2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RDNT-00001</t>
+    <t>ELEC-ELEC-STD-ORDNTR-AAAA</t>
   </si>
   <si>
     <t>K700-SE-2</t>
@@ -2123,7 +2123,7 @@
     <t>CPU1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-PNTS-00001</t>
+    <t>ELEC-ELEC-STD-PONTS-AAAA</t>
   </si>
   <si>
     <t>FBS 2-5</t>
@@ -2141,7 +2141,7 @@
     <t>TBBR1, TBBR3, TBBR5</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-PNTS-00002</t>
+    <t>ELEC-ELEC-STD-PONTS-AAAB</t>
   </si>
   <si>
     <t>FBS 3-5</t>
@@ -2156,7 +2156,7 @@
     <t>TBBR2, TBBR4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-PRT--00001</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAQ</t>
   </si>
   <si>
     <t>03540503Z</t>
@@ -2171,7 +2171,7 @@
     <t>FH3, FH4, FH5, FH6</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-PRT--00002</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAR</t>
   </si>
   <si>
     <t>04980933.X</t>
@@ -2183,7 +2183,7 @@
     <t>FH2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-PRT--00003</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAS</t>
   </si>
   <si>
     <t>15600-04-20</t>
@@ -2195,7 +2195,7 @@
     <t>FH7</t>
   </si>
   <si>
-    <t>ELEC-ELEC-FUSE-PRT--00004</t>
+    <t>ELEC-ELEC-FUSE-FUSIBL-AAAT</t>
   </si>
   <si>
     <t>5073550</t>
@@ -2207,7 +2207,7 @@
     <t>FH1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RLST-00001</t>
+    <t>ELEC-ELEC-STD-RELAIS-AAAA</t>
   </si>
   <si>
     <t>2900932</t>
@@ -2222,7 +2222,7 @@
     <t>KB1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RLST-00002</t>
+    <t>ELEC-ELEC-STD-RELAIS-AAAB</t>
   </si>
   <si>
     <t>2903661</t>
@@ -2234,7 +2234,7 @@
     <t>K1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RLST-00003</t>
+    <t>ELEC-ELEC-STD-RELAIS-AAAC</t>
   </si>
   <si>
     <t>A21CSQ24VDC1.6</t>
@@ -2249,7 +2249,7 @@
     <t>K5, K6</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RLST-00004</t>
+    <t>ELEC-ELEC-STD-RELAIS-AAAD</t>
   </si>
   <si>
     <t>AEV250-MA</t>
@@ -2264,7 +2264,7 @@
     <t>K2, K3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RLST-00005</t>
+    <t>ELEC-ELEC-STD-RELAIS-AAAE</t>
   </si>
   <si>
     <t>DCNEV150-MA</t>
@@ -2276,7 +2276,7 @@
     <t>K4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RSST-00001</t>
+    <t>ELEC-ELEC-STD-RESIST-AAAA</t>
   </si>
   <si>
     <t>RNMF14FTC120R</t>
@@ -2291,7 +2291,7 @@
     <t>R1, R2, R3, R4, R5, R7, R8, R9</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RFXX-00001</t>
+    <t>ELEC-ELEC-STD-RF-AAAA</t>
   </si>
   <si>
     <t>095-902-535M200</t>
@@ -2309,7 +2309,7 @@
     <t>WH35</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RFXX-00002</t>
+    <t>ELEC-ELEC-STD-RF-AAAB</t>
   </si>
   <si>
     <t>095-902-536-036</t>
@@ -2321,7 +2321,7 @@
     <t>WH34</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RFXX-00003</t>
+    <t>ELEC-ELEC-STD-RF-AAAC</t>
   </si>
   <si>
     <t>095-902-536-048</t>
@@ -2333,7 +2333,7 @@
     <t>WH3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-SLCT-00001</t>
+    <t>ELEC-ELEC-STD-SLCTRS-AAAA</t>
   </si>
   <si>
     <t>35-210-051-R-900</t>
@@ -2348,7 +2348,7 @@
     <t>S1</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-SLCT-00002</t>
+    <t>ELEC-ELEC-STD-SLCTRS-AAAB</t>
   </si>
   <si>
     <t>XB7NG21</t>
@@ -2360,7 +2360,7 @@
     <t>S4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00001</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAA</t>
   </si>
   <si>
     <t>110G18</t>
@@ -2375,7 +2375,7 @@
     <t>MEC1, MEC2</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00002</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAB</t>
   </si>
   <si>
     <t>110G19</t>
@@ -2387,7 +2387,7 @@
     <t>MEC3, MEC4, MEC5, MEC6, MEC7</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00003</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAC</t>
   </si>
   <si>
     <t>W12P</t>
@@ -2399,7 +2399,7 @@
     <t>WD26, WD29</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00004</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAD</t>
   </si>
   <si>
     <t>W12S</t>
@@ -2411,7 +2411,7 @@
     <t>WD6, WD7, WD30</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00005</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAE</t>
   </si>
   <si>
     <t>W2P</t>
@@ -2423,7 +2423,7 @@
     <t>WD13, WD16, WD17, WD19, WD22</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00006</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAF</t>
   </si>
   <si>
     <t>W2S</t>
@@ -2435,7 +2435,7 @@
     <t>WD12, WD14, WD15, WD18, WD23</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00007</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAG</t>
   </si>
   <si>
     <t>W4P</t>
@@ -2447,7 +2447,7 @@
     <t>WD24</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00008</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAH</t>
   </si>
   <si>
     <t>W6P</t>
@@ -2459,7 +2459,7 @@
     <t>WD9, WD11, WD21</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00009</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAJ</t>
   </si>
   <si>
     <t>W6S</t>
@@ -2471,7 +2471,7 @@
     <t>WD8, WD10, WD20</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00010</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAK</t>
   </si>
   <si>
     <t>W8P</t>
@@ -2483,7 +2483,7 @@
     <t>WD25, WD27, WD28</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00011</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAM</t>
   </si>
   <si>
     <t>WM12P</t>
@@ -2495,7 +2495,7 @@
     <t>WD1, WD3</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-VRRS-00012</t>
+    <t>ELEC-ELEC-STD-VRROSE-AAAN</t>
   </si>
   <si>
     <t>WM12S</t>
@@ -2507,7 +2507,7 @@
     <t>WD2, WD4</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-181P-00001</t>
+    <t>MECA-MECA-STD-383PLQ-AAAA</t>
   </si>
   <si>
     <t>D-0054459</t>
@@ -2525,7 +2525,7 @@
     <t>MÉCANIQUE</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-181P-00002</t>
+    <t>MECA-MECA-STD-383PLQ-AAAB</t>
   </si>
   <si>
     <t>D-0055553</t>
@@ -2534,7 +2534,7 @@
     <t>ID_TAG AMR-PL-4650-aau02####</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-181P-00003</t>
+    <t>MECA-MECA-STD-383PLQ-AAAC</t>
   </si>
   <si>
     <t>D-0055554</t>
@@ -2543,7 +2543,7 @@
     <t>BATTERY_TAG</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-180É-00001</t>
+    <t>MECA-MECA-STD-382TQT-AAAA</t>
   </si>
   <si>
     <t>D-0055524</t>
@@ -2555,7 +2555,7 @@
     <t>180 | ÉTIQUETTES</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-180É-00002</t>
+    <t>MECA-MECA-STD-382TQT-AAAB</t>
   </si>
   <si>
     <t>D-0055527</t>
@@ -2564,7 +2564,7 @@
     <t>AUTOCOLLANT NE PAS MONTER 1-1/2''</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-180É-00003</t>
+    <t>MECA-MECA-STD-382TQT-AAAC</t>
   </si>
   <si>
     <t>D-0055529</t>
@@ -2573,7 +2573,7 @@
     <t>AUTOCOLLANT NOOVELIA 1-5/16" x 8"'</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-180É-00004</t>
+    <t>MECA-MECA-STD-382TQT-AAAD</t>
   </si>
   <si>
     <t>D-0055530</t>
@@ -2582,7 +2582,7 @@
     <t>AUTOCOLLANT PENTE ET VOLTAGE</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-180É-00005</t>
+    <t>MECA-MECA-STD-382TQT-AAAE</t>
   </si>
   <si>
     <t>D-0055531</t>
@@ -2591,7 +2591,7 @@
     <t>AUTOCOLLANT POINT DE LEVAGE 1-1/4''</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-180É-00006</t>
+    <t>MECA-MECA-STD-382TQT-AAAF</t>
   </si>
   <si>
     <t>D-0055534</t>
@@ -2600,7 +2600,7 @@
     <t>AUTOCOLLANT VÉHICULE AUTOMATIQUE 38MM</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-180É-00007</t>
+    <t>MECA-MECA-STD-382TQT-AAAG</t>
   </si>
   <si>
     <t>D-0055539</t>
@@ -2609,7 +2609,7 @@
     <t>DÉPART/ARRÊT</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-180É-00008</t>
+    <t>MECA-MECA-STD-382TQT-AAAH</t>
   </si>
   <si>
     <t>D-0055540</t>
@@ -2618,7 +2618,7 @@
     <t>DANGER ÉLECTRIQUE 60V 1''</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-140F-00001</t>
+    <t>MECA-MECA-STD-342FBR-AAAA</t>
   </si>
   <si>
     <t>D-0050448</t>
@@ -2630,7 +2630,7 @@
     <t>140 | FABRICATION ADDITIVE</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-140F-00002</t>
+    <t>MECA-MECA-STD-342FBR-AAAB</t>
   </si>
   <si>
     <t>D-0055091</t>
@@ -2639,7 +2639,7 @@
     <t>DOUBLE MODULE VIDE</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-140F-00003</t>
+    <t>MECA-MECA-STD-342FBR-AAAC</t>
   </si>
   <si>
     <t>D-0055151</t>
@@ -2648,7 +2648,7 @@
     <t>PASSE-PAROI IMPRIMÉ POUR PP75</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-140F-00004</t>
+    <t>MECA-MECA-STD-342FBR-AAAD</t>
   </si>
   <si>
     <t>D-0055164</t>
@@ -2657,7 +2657,7 @@
     <t>COUVERCLE POUR CONNECTEUR DE RECHARGE</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-140F-00005</t>
+    <t>MECA-MECA-STD-342FBR-AAAE</t>
   </si>
   <si>
     <t>D-0055167</t>
@@ -2666,7 +2666,7 @@
     <t>SUPPORT CONNECTEUR DE RECHARGE</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-140F-00006</t>
+    <t>MECA-MECA-STD-342FBR-AAAF</t>
   </si>
   <si>
     <t>D-0055261</t>
@@ -2675,7 +2675,7 @@
     <t>CAPUCHON POUR CONNECTEUR DEUTSCH 8 PINS</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-140F-00007</t>
+    <t>MECA-MECA-STD-342FBR-AAAG</t>
   </si>
   <si>
     <t>D-0055263</t>
@@ -2684,7 +2684,7 @@
     <t>CAPUCHON POUR CONNECTEUR DEUTSCH 4 PINS</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-140F-00008</t>
+    <t>MECA-MECA-STD-342FBR-AAAH</t>
   </si>
   <si>
     <t>D-0055333</t>
@@ -2693,7 +2693,7 @@
     <t>PI - BOITIER DEL DEUTSCH ET RAIL DIN VERTICAL</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00001</t>
+    <t>MECA-MACH-MILL-USINER-AAAA</t>
   </si>
   <si>
     <t>A-0008981</t>
@@ -2705,7 +2705,7 @@
     <t>131 | PIÈCES USINÉES</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00002</t>
+    <t>MECA-MACH-MILL-USINER-AAAB</t>
   </si>
   <si>
     <t>A-0009800</t>
@@ -2714,7 +2714,7 @@
     <t>CHÂSSIS PL4650-V2</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00003</t>
+    <t>MECA-MACH-MILL-USINER-AAAC</t>
   </si>
   <si>
     <t>A-0009856</t>
@@ -2723,7 +2723,7 @@
     <t>BRAS DE SUSPENSION - CORPS PIVOT USINÉ GAUCHE</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00004</t>
+    <t>MECA-MACH-MILL-USINER-AAAD</t>
   </si>
   <si>
     <t>A-0009857</t>
@@ -2732,7 +2732,7 @@
     <t>BRAS DE SUSPENSION - CORPS PIVOT USINÉ DROIT</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00005</t>
+    <t>MECA-MACH-MILL-USINER-AAAE</t>
   </si>
   <si>
     <t>D-0049716</t>
@@ -2741,7 +2741,7 @@
     <t>ARBRE PIVOT SUSPENSION</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00006</t>
+    <t>MECA-MACH-MILL-USINER-AAAF</t>
   </si>
   <si>
     <t>D-0049717</t>
@@ -2750,7 +2750,7 @@
     <t>PALIER PIVOT SUSPENSION</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00007</t>
+    <t>MECA-MACH-MILL-USINER-AAAG</t>
   </si>
   <si>
     <t>D-0049718</t>
@@ -2759,7 +2759,7 @@
     <t>CALLE PALIER PIVOT SUSPENSION</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00008</t>
+    <t>MECA-MACH-MILL-USINER-AAAH</t>
   </si>
   <si>
     <t>D-0050086</t>
@@ -2768,7 +2768,7 @@
     <t>BUTÉE ROULEMENT PIVOT SUSPENSION</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00009</t>
+    <t>MECA-MACH-MILL-USINER-AAAJ</t>
   </si>
   <si>
     <t>D-0050417</t>
@@ -2777,7 +2777,7 @@
     <t>BT - SUPPORT BOBINE DE RECHARGE</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00010</t>
+    <t>MECA-MACH-MILL-USINER-AAAK</t>
   </si>
   <si>
     <t>D-0053683</t>
@@ -2786,7 +2786,7 @@
     <t>PLAQUETTE ADAPTEUR ENCODEUR SAFETY</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00011</t>
+    <t>MECA-MACH-MILL-USINER-AAAM</t>
   </si>
   <si>
     <t>D-0053993</t>
@@ -2795,7 +2795,7 @@
     <t>PLAQUE SUPPORT SUSPENSION V2</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00012</t>
+    <t>MECA-MACH-MILL-USINER-AAAN</t>
   </si>
   <si>
     <t>D-0054318</t>
@@ -2804,7 +2804,7 @@
     <t>BRAS DE SUSPENSION - MOTEUR GAUCHE</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00013</t>
+    <t>MECA-MACH-MILL-USINER-AAAP</t>
   </si>
   <si>
     <t>D-0054322</t>
@@ -2813,7 +2813,7 @@
     <t>BRAS DE SUSPENSION - MOTEUR DROIT</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00014</t>
+    <t>MECA-MACH-MILL-USINER-AAAQ</t>
   </si>
   <si>
     <t>D-0054448</t>
@@ -2822,7 +2822,7 @@
     <t>CIBLE FIXATION MAGNÉTIQUE CARROSSERIE</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00015</t>
+    <t>MECA-MACH-MILL-USINER-AAAR</t>
   </si>
   <si>
     <t>D-0054735</t>
@@ -2831,7 +2831,7 @@
     <t>ESPACEUR POUR ROULETTE</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00016</t>
+    <t>MECA-MACH-MILL-USINER-AAAS</t>
   </si>
   <si>
     <t>D-0055358</t>
@@ -2840,7 +2840,7 @@
     <t>SUPPORT HAUT ISOLANT POUR ORDINATEUR</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00017</t>
+    <t>MECA-MACH-MILL-USINER-AAAT</t>
   </si>
   <si>
     <t>D-0055359</t>
@@ -2849,7 +2849,7 @@
     <t>SUPPORT BAS ISOLANT POUR ORDINATEUR</t>
   </si>
   <si>
-    <t>MECA-MACH-MILL-131P-00018</t>
+    <t>MECA-MACH-MILL-USINER-AAAW</t>
   </si>
   <si>
     <t>D-0055961</t>
@@ -2858,7 +2858,7 @@
     <t>SPACER LECTEUR MAGNÉTIQUE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00001</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAA</t>
   </si>
   <si>
     <t>D-0050007</t>
@@ -2870,7 +2870,7 @@
     <t>121 | PIÈCES PLIÉES</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00002</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAB</t>
   </si>
   <si>
     <t>D-0050018</t>
@@ -2879,7 +2879,7 @@
     <t>RENFORT EXTÉRIEUR ARRIÈRE - TÔLE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00003</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAC</t>
   </si>
   <si>
     <t>D-0050077</t>
@@ -2888,7 +2888,7 @@
     <t>RENFORT INTERNE ARRIÈRE - TÔLE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00004</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAD</t>
   </si>
   <si>
     <t>D-0050131</t>
@@ -2897,7 +2897,7 @@
     <t>CAPAGE ROUE LIBRE AVANT</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00005</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAE</t>
   </si>
   <si>
     <t>D-0050316</t>
@@ -2906,7 +2906,7 @@
     <t>BRACKET CARROSSERIE PL - COIN BAS</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00006</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAF</t>
   </si>
   <si>
     <t>D-0050413</t>
@@ -2915,7 +2915,7 @@
     <t>BT - CÔTÉ</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00007</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAG</t>
   </si>
   <si>
     <t>D-0050416</t>
@@ -2924,7 +2924,7 @@
     <t>BT - SUPPORT BATTERIES</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00008</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAH</t>
   </si>
   <si>
     <t>D-0050420</t>
@@ -2933,7 +2933,7 @@
     <t>BT - CROCHET DE LEVAGE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00009</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAJ</t>
   </si>
   <si>
     <t>D-0051124</t>
@@ -2942,7 +2942,7 @@
     <t>SUPPORT POUR CARROSSERIE CÔTÉ BAS</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00010</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAK</t>
   </si>
   <si>
     <t>D-0053995</t>
@@ -2951,7 +2951,7 @@
     <t>CHÂSSIS V2 - INTÉRIEUR CENTRE GAUCHE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00011</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAM</t>
   </si>
   <si>
     <t>D-0053997</t>
@@ -2960,7 +2960,7 @@
     <t>CHÂSSIS V2 - CADRE FIXE GAUCHE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00012</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAN</t>
   </si>
   <si>
     <t>D-0053998</t>
@@ -2969,7 +2969,7 @@
     <t>CHÂSSIS V2 - INTÉRIEUR CENTRE DROIT</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00013</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAP</t>
   </si>
   <si>
     <t>D-0053999</t>
@@ -2978,7 +2978,7 @@
     <t>CHÂSSIS V2 - CADRE FIXE DROIT</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00014</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAQ</t>
   </si>
   <si>
     <t>D-0054001</t>
@@ -2987,7 +2987,7 @@
     <t>SUPPORT BALAYEUR LASER - PIÈCE MOBILE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00015</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAR</t>
   </si>
   <si>
     <t>D-0054007</t>
@@ -2996,7 +2996,7 @@
     <t>PLAQUE DE FOND CÔTÉ</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00016</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAS</t>
   </si>
   <si>
     <t>D-0054008</t>
@@ -3005,7 +3005,7 @@
     <t>CHÂSSIS V2 - CADRE ARRIÈRE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00017</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAT</t>
   </si>
   <si>
     <t>D-0054009</t>
@@ -3014,7 +3014,7 @@
     <t>CHÂSSIS V2 - CADRE AVANT</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00018</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAW</t>
   </si>
   <si>
     <t>D-0054010</t>
@@ -3023,7 +3023,7 @@
     <t>CHÂSSIS V2 - PIÈCE CENTRALE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00019</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAX</t>
   </si>
   <si>
     <t>D-0054029</t>
@@ -3032,7 +3032,7 @@
     <t>BRACKET CARROSSERIE PL - COIN HAUT 1B</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00020</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAY</t>
   </si>
   <si>
     <t>D-0054031</t>
@@ -3041,7 +3041,7 @@
     <t>CHÂSSIS V2 - INTÉRIEUR AVANT GAUCHE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00021</t>
+    <t>MECA-STD-BEND-PLIAGE-AAAZ</t>
   </si>
   <si>
     <t>D-0054042</t>
@@ -3050,7 +3050,7 @@
     <t>CHÂSSIS V2 - INTÉRIEUR AVANT DROIT</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00022</t>
+    <t>MECA-STD-BEND-PLIAGE-AAA2</t>
   </si>
   <si>
     <t>D-0054092</t>
@@ -3059,7 +3059,7 @@
     <t>CHÂSSIS V2 - CAPAGE ENCODEUR</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00023</t>
+    <t>MECA-STD-BEND-PLIAGE-AAA3</t>
   </si>
   <si>
     <t>D-0054253</t>
@@ -3068,7 +3068,7 @@
     <t>SUPPORT BALAYEUR LASER - PIÈCE FIXE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00024</t>
+    <t>MECA-STD-BEND-PLIAGE-AAA4</t>
   </si>
   <si>
     <t>D-0054269</t>
@@ -3077,7 +3077,7 @@
     <t>RENFORT EXTERNE CÔTÉ - TÔLE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00025</t>
+    <t>MECA-STD-BEND-PLIAGE-AAA5</t>
   </si>
   <si>
     <t>D-0054272</t>
@@ -3086,7 +3086,7 @@
     <t>CHÂSSIS V2 - INTÉRIEUR ARRIÈRE DROIT</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00026</t>
+    <t>MECA-STD-BEND-PLIAGE-AAA6</t>
   </si>
   <si>
     <t>D-0054273</t>
@@ -3095,7 +3095,7 @@
     <t>CHÂSSIS V2 - INTÉRIEUR ARRIÈRE GAUCHE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00027</t>
+    <t>MECA-STD-BEND-PLIAGE-AAA7</t>
   </si>
   <si>
     <t>D-0054278</t>
@@ -3104,7 +3104,7 @@
     <t>BRACKET CARROSSERIE PL - COIN HAUT 1A</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00028</t>
+    <t>MECA-STD-BEND-PLIAGE-AAA8</t>
   </si>
   <si>
     <t>D-0054279</t>
@@ -3113,7 +3113,7 @@
     <t>BRACKET CARROSSERIE PL - COIN HAUT 2A</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00029</t>
+    <t>MECA-STD-BEND-PLIAGE-AAA9</t>
   </si>
   <si>
     <t>D-0054284</t>
@@ -3122,7 +3122,7 @@
     <t>BRACKET CARROSSERIE PL - CÔTÉ HAUT 1A</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00030</t>
+    <t>MECA-STD-BEND-PLIAGE-AABA</t>
   </si>
   <si>
     <t>D-0054285</t>
@@ -3131,7 +3131,7 @@
     <t>BRACKET CARROSSERIE PL - CÔTÉ HAUT 2A</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00031</t>
+    <t>MECA-STD-BEND-PLIAGE-AABB</t>
   </si>
   <si>
     <t>D-0054287</t>
@@ -3140,7 +3140,7 @@
     <t>BRACKET CARROSSERIE PL - CÔTÉ HAUT 1B</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00032</t>
+    <t>MECA-STD-BEND-PLIAGE-AABC</t>
   </si>
   <si>
     <t>D-0054288</t>
@@ -3149,7 +3149,7 @@
     <t>BRACKET CARROSSERIE PL - CÔTÉ HAUT 2B</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00033</t>
+    <t>MECA-STD-BEND-PLIAGE-AABD</t>
   </si>
   <si>
     <t>D-0054292</t>
@@ -3158,7 +3158,7 @@
     <t>BRACKET CARROSSERIE PL - COIN HAUT 2B</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00034</t>
+    <t>MECA-STD-BEND-PLIAGE-AABE</t>
   </si>
   <si>
     <t>D-0054295</t>
@@ -3167,7 +3167,7 @@
     <t>PLAQUE ÉLECTRIQUE ARRIÈRE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00035</t>
+    <t>MECA-STD-BEND-PLIAGE-AABF</t>
   </si>
   <si>
     <t>D-0054296</t>
@@ -3176,7 +3176,7 @@
     <t>SUPPORT PLAQUE ÉLECTRIQUE ARRIÈRE 1</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00036</t>
+    <t>MECA-STD-BEND-PLIAGE-AABG</t>
   </si>
   <si>
     <t>D-0054297</t>
@@ -3185,7 +3185,7 @@
     <t>SUPPORT PLAQUE ÉLECTRIQUE ARRIÈRE 2</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00037</t>
+    <t>MECA-STD-BEND-PLIAGE-AABH</t>
   </si>
   <si>
     <t>D-0054301</t>
@@ -3194,7 +3194,7 @@
     <t>PLAQUE DIAGNOSTIQUE ÉLECTRIQUE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00038</t>
+    <t>MECA-STD-BEND-PLIAGE-AABJ</t>
   </si>
   <si>
     <t>D-0054310</t>
@@ -3203,7 +3203,7 @@
     <t>SUPPORT RFID</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00039</t>
+    <t>MECA-STD-BEND-PLIAGE-AABK</t>
   </si>
   <si>
     <t>D-0054317</t>
@@ -3212,7 +3212,7 @@
     <t>SUPPORT LECTEUR MAGNÉTIQUE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00040</t>
+    <t>MECA-STD-BEND-PLIAGE-AABM</t>
   </si>
   <si>
     <t>D-0054325</t>
@@ -3221,7 +3221,7 @@
     <t>SUPPORT À GOULOTTE COIN EXTÉRIEUR</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00041</t>
+    <t>MECA-STD-BEND-PLIAGE-AABN</t>
   </si>
   <si>
     <t>D-0054957</t>
@@ -3230,7 +3230,7 @@
     <t>SUPPORT CONNECTEUR 2X PP180</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00042</t>
+    <t>MECA-STD-BEND-PLIAGE-AABP</t>
   </si>
   <si>
     <t>D-0054986</t>
@@ -3239,7 +3239,7 @@
     <t>ÉQUERRE DE CADENASSAGE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00043</t>
+    <t>MECA-STD-BEND-PLIAGE-AABQ</t>
   </si>
   <si>
     <t>D-0055093</t>
@@ -3248,7 +3248,7 @@
     <t>BOITIER ÉLEC. - PLAQUE DE FOND</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00044</t>
+    <t>MECA-STD-BEND-PLIAGE-AABR</t>
   </si>
   <si>
     <t>D-0055095</t>
@@ -3257,7 +3257,7 @@
     <t>BOITIER ÉLEC. - CÔTÉ GAUCHE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00045</t>
+    <t>MECA-STD-BEND-PLIAGE-AABS</t>
   </si>
   <si>
     <t>D-0055098</t>
@@ -3266,7 +3266,7 @@
     <t>BOITIER ÉLEC. - CÔTÉ DROIT</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00046</t>
+    <t>MECA-STD-BEND-PLIAGE-AABT</t>
   </si>
   <si>
     <t>D-0055103</t>
@@ -3275,7 +3275,7 @@
     <t>BOITIER ÉLEC. - TABLETTE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00047</t>
+    <t>MECA-STD-BEND-PLIAGE-AABW</t>
   </si>
   <si>
     <t>D-0055106</t>
@@ -3284,7 +3284,7 @@
     <t>BOITIER ÉLEC. - MONTANT TABLETTE</t>
   </si>
   <si>
-    <t>MECA-BEND-BEND-121P-00048</t>
+    <t>MECA-STD-BEND-PLIAGE-AABX</t>
   </si>
   <si>
     <t>D-0058161</t>
@@ -3293,7 +3293,7 @@
     <t>PENTURE POUR RELAIS ET BORNIER</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-112P-00001</t>
+    <t>MECA-MECA-STD-DECOUP-AAAA</t>
   </si>
   <si>
     <t>D-0050065</t>
@@ -3305,7 +3305,7 @@
     <t>112 | PIÈCES DÉCOUPÉES SCIE</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00001</t>
+    <t>MECA-LASER-STD-DECOUP-AAAA</t>
   </si>
   <si>
     <t>D-0049970</t>
@@ -3317,7 +3317,7 @@
     <t>111 | PIÈCES DÉCOUPÉES LASER</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00002</t>
+    <t>MECA-LASER-STD-DECOUP-AAAB</t>
   </si>
   <si>
     <t>D-0049971</t>
@@ -3326,7 +3326,7 @@
     <t>BRAS DE SUSPENSION - RENFORT ROUE LIBRE</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00003</t>
+    <t>MECA-LASER-STD-DECOUP-AAAC</t>
   </si>
   <si>
     <t>D-0050046</t>
@@ -3335,7 +3335,7 @@
     <t>BRAS DE SUSPENSION ARRIÈRE - CORPS PIVOT</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00004</t>
+    <t>MECA-LASER-STD-DECOUP-AAAD</t>
   </si>
   <si>
     <t>D-0050132</t>
@@ -3344,7 +3344,7 @@
     <t>RONDELLE DE SERRAGE AXIAL PIVOT</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00005</t>
+    <t>MECA-LASER-STD-DECOUP-AAAE</t>
   </si>
   <si>
     <t>D-0050412</t>
@@ -3353,7 +3353,7 @@
     <t>BT - PLAQUE DE FOND</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00006</t>
+    <t>MECA-LASER-STD-DECOUP-AAAF</t>
   </si>
   <si>
     <t>D-0050414</t>
@@ -3362,7 +3362,7 @@
     <t>BT - SÉPARATEUR 1</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00007</t>
+    <t>MECA-LASER-STD-DECOUP-AAAG</t>
   </si>
   <si>
     <t>D-0050415</t>
@@ -3371,7 +3371,7 @@
     <t>BT - SÉPARATEUR MILIEU</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00008</t>
+    <t>MECA-LASER-STD-DECOUP-AAAH</t>
   </si>
   <si>
     <t>D-0050419</t>
@@ -3380,7 +3380,7 @@
     <t>BT - PIÈCE VISSAGE SUPPORT BOBINE</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00009</t>
+    <t>MECA-LASER-STD-DECOUP-AAAJ</t>
   </si>
   <si>
     <t>D-0051088</t>
@@ -3389,7 +3389,7 @@
     <t>BRACKET CARROSSERIE PL - CÔTÉ BAS</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00010</t>
+    <t>MECA-LASER-STD-DECOUP-AAAK</t>
   </si>
   <si>
     <t>D-0053996</t>
@@ -3398,7 +3398,7 @@
     <t>CHÂSSIS V2 - PLAQUE DE FOND</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00011</t>
+    <t>MECA-LASER-STD-DECOUP-AAAM</t>
   </si>
   <si>
     <t>D-0054298</t>
@@ -3407,7 +3407,7 @@
     <t>PLAQUE PASSE PAROI - BATTERIE</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00012</t>
+    <t>MECA-LASER-STD-DECOUP-AAAN</t>
   </si>
   <si>
     <t>D-0054299</t>
@@ -3416,7 +3416,7 @@
     <t>PLAQUE PASSE PAROI - MOTEUR CENTRE</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00013</t>
+    <t>MECA-LASER-STD-DECOUP-AAAP</t>
   </si>
   <si>
     <t>D-0054300</t>
@@ -3425,7 +3425,7 @@
     <t>PLAQUE PASSE PAROI - MOTEUR CÔTÉ</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00014</t>
+    <t>MECA-LASER-STD-DECOUP-AAAQ</t>
   </si>
   <si>
     <t>D-0054307</t>
@@ -3434,7 +3434,7 @@
     <t>PLAQUE PASSE PAROI - CÔTÉ EXT. AV.</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00015</t>
+    <t>MECA-LASER-STD-DECOUP-AAAR</t>
   </si>
   <si>
     <t>D-0054308</t>
@@ -3443,7 +3443,7 @@
     <t>PLAQUE PASSE PAROI - CÔTÉ EXT. ARR.</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00016</t>
+    <t>MECA-LASER-STD-DECOUP-AAAS</t>
   </si>
   <si>
     <t>D-0054309</t>
@@ -3452,7 +3452,7 @@
     <t>PLAQUE PASSE PAROI - AVANT INTÉRIEUR</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00017</t>
+    <t>MECA-LASER-STD-DECOUP-AAAT</t>
   </si>
   <si>
     <t>D-0054320</t>
@@ -3461,7 +3461,7 @@
     <t>BRAS DE SUSPENSION - CORPS PIVOT</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00018</t>
+    <t>MECA-LASER-STD-DECOUP-AAAW</t>
   </si>
   <si>
     <t>D-0054982</t>
@@ -3470,7 +3470,7 @@
     <t>SUPPORT D'INTERFACE POUR DISJONCTEUR</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00019</t>
+    <t>MECA-LASER-STD-DECOUP-AAAX</t>
   </si>
   <si>
     <t>D-0055284</t>
@@ -3479,7 +3479,7 @@
     <t>PLAQUE ADAPTEUR ENCODEUR MOTEUR</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00020</t>
+    <t>MECA-LASER-STD-DECOUP-AAAY</t>
   </si>
   <si>
     <t>D-0055405</t>
@@ -3488,7 +3488,7 @@
     <t>PLAQUE GAUCHE COMPOSANTS BATTERIE</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00021</t>
+    <t>MECA-LASER-STD-DECOUP-AAAZ</t>
   </si>
   <si>
     <t>D-0055406</t>
@@ -3497,7 +3497,7 @@
     <t>PLAQUE DE FOND POUR COMPOSANT BATTERIE</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00022</t>
+    <t>MECA-LASER-STD-DECOUP-AAA2</t>
   </si>
   <si>
     <t>D-0055407</t>
@@ -3506,7 +3506,7 @@
     <t>PLAQUE ARRIÈRE COMPOSANTS BATTERIE</t>
   </si>
   <si>
-    <t>MECA-LASER-CUT-111P-00023</t>
+    <t>MECA-LASER-STD-DECOUP-AAA3</t>
   </si>
   <si>
     <t>D-0055408</t>
@@ -3515,7 +3515,7 @@
     <t>PLAQUE DROITE COMPOSANTS BATTERIE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-103S-00001</t>
+    <t>MECA-ASS-STD-323SSM-AAAA</t>
   </si>
   <si>
     <t>A-0009055</t>
@@ -3527,7 +3527,7 @@
     <t>103 | ASSEMBLAGE FOURNISSEUR</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-103S-00002</t>
+    <t>MECA-ASS-STD-323SSM-AAAB</t>
   </si>
   <si>
     <t>A-0009057</t>
@@ -3536,7 +3536,7 @@
     <t>CARROSSERIE PL - ASS. CÔTÉ BAS - LG 6</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-103S-00003</t>
+    <t>MECA-ASS-STD-323SSM-AAAC</t>
   </si>
   <si>
     <t>A-0009059</t>
@@ -3545,7 +3545,7 @@
     <t>CARROSSERIE PL - ASS. CÔTÉ BAS - LG 4</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-103S-00004</t>
+    <t>MECA-ASS-STD-323SSM-AAAD</t>
   </si>
   <si>
     <t>A-0009081</t>
@@ -3554,7 +3554,7 @@
     <t>CARROSSERIE PL - ASS. COIN BAS SANS BALAYEUR</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-103S-00005</t>
+    <t>MECA-ASS-STD-323SSM-AAAE</t>
   </si>
   <si>
     <t>A-0009807</t>
@@ -3563,7 +3563,7 @@
     <t>CARROSSERIE PLx6 - ASS. CÔTÉ HAUT</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-103S-00006</t>
+    <t>MECA-ASS-STD-323SSM-AAAF</t>
   </si>
   <si>
     <t>A-0009808</t>
@@ -3572,7 +3572,7 @@
     <t>CARROSSERIE PL4x - ASS. ARRIÈRE HAUT</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-103S-00007</t>
+    <t>MECA-ASS-STD-323SSM-AAAG</t>
   </si>
   <si>
     <t>A-0009809</t>
@@ -3581,7 +3581,7 @@
     <t>CARROSSERIE PL4x - ASS. AVANT HAUT</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-103S-00008</t>
+    <t>MECA-ASS-STD-323SSM-AAAH</t>
   </si>
   <si>
     <t>A-0009815</t>
@@ -3590,7 +3590,7 @@
     <t>CARROSSERIE PL - ASS. COIN HAUT</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-025Q-00001</t>
+    <t>MECA-MECA-STD-225QNC-AAAA</t>
   </si>
   <si>
     <t>MUSB2E151015BP</t>
@@ -3605,7 +3605,7 @@
     <t>AMPHENOL</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-025Q-00002</t>
+    <t>MECA-MECA-STD-225QNC-AAAB</t>
   </si>
   <si>
     <t>1464G2</t>
@@ -3617,7 +3617,7 @@
     <t>ANDERSON</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-025Q-00003</t>
+    <t>MECA-MECA-STD-225QNC-AAAC</t>
   </si>
   <si>
     <t>CP-RJ45</t>
@@ -3629,7 +3629,7 @@
     <t>MOUSER</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-025Q-00004</t>
+    <t>MECA-MECA-STD-225QNC-AAAD</t>
   </si>
   <si>
     <t>726851001</t>
@@ -3641,7 +3641,7 @@
     <t>WURTH ELEKTRONIK</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-023C-00001</t>
+    <t>MECA-MECA-STD-223COM-AAAA</t>
   </si>
   <si>
     <t>03540519Z</t>
@@ -3656,7 +3656,7 @@
     <t>LITTELFUSE</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-023C-00002</t>
+    <t>MECA-MECA-STD-223COM-AAAB</t>
   </si>
   <si>
     <t>03540523Z</t>
@@ -3665,7 +3665,7 @@
     <t>VERROU DE BLOC MODULAIRE LITTELFUSE</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00001</t>
+    <t>MECA-MECA-STD-COMPNT-AAAA</t>
   </si>
   <si>
     <t>GR3250A</t>
@@ -3680,7 +3680,7 @@
     <t>ESSENTRA COMPONENTS</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00002</t>
+    <t>MECA-MECA-STD-COMPNT-AAAB</t>
   </si>
   <si>
     <t>S-ZFHS-5DB70</t>
@@ -3692,7 +3692,7 @@
     <t>HAMILTON CASTERS</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00003</t>
+    <t>MECA-MECA-STD-COMPNT-AAAC</t>
   </si>
   <si>
     <t>5862K107</t>
@@ -3704,7 +3704,7 @@
     <t>MCMASTER</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00004</t>
+    <t>MECA-MECA-STD-COMPNT-AAAD</t>
   </si>
   <si>
     <t>7565K77</t>
@@ -3713,7 +3713,7 @@
     <t>PUSH IN CABLE HOLDER, 1" BUNDLE, FOR Ø1/4" X MAX 3/8"</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00005</t>
+    <t>MECA-MECA-STD-COMPNT-AAAE</t>
   </si>
   <si>
     <t>8510k22</t>
@@ -3722,7 +3722,7 @@
     <t>RUBBER TRIM 1/4 X 5/16</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00006</t>
+    <t>MECA-MECA-STD-COMPNT-AAAF</t>
   </si>
   <si>
     <t>90692A719</t>
@@ -3731,7 +3731,7 @@
     <t>SLOTTED SPRING PIN, Ø3/16 X 3/8 LG, ZINC PLATED STEEL</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00007</t>
+    <t>MECA-MECA-STD-COMPNT-AAAG</t>
   </si>
   <si>
     <t>90720A460</t>
@@ -3740,7 +3740,7 @@
     <t>RIVET ÉCROU ANTI-ROTATION 1/4-20 POUR 0.085-0.145"ÉP.</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00008</t>
+    <t>MECA-MECA-STD-COMPNT-AAAH</t>
   </si>
   <si>
     <t>9309K57</t>
@@ -3749,7 +3749,7 @@
     <t>PUSH-IN BUMPER 3/8" H X 15/64" ID</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00009</t>
+    <t>MECA-MECA-STD-COMPNT-AAAJ</t>
   </si>
   <si>
     <t>93275K127</t>
@@ -3758,7 +3758,7 @@
     <t>BANDE DE MOUSSE POLYURÉTHANE, AUTOCOLLANTE, 1/8 ÉP. 3/8 LRG.</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00010</t>
+    <t>MECA-MECA-STD-COMPNT-AAAK</t>
   </si>
   <si>
     <t>93560A180</t>
@@ -3767,7 +3767,7 @@
     <t>ÉCROU À SOUDER 1/2"-13 UNC</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00011</t>
+    <t>MECA-MECA-STD-COMPNT-AAAM</t>
   </si>
   <si>
     <t>93886A140</t>
@@ -3776,7 +3776,7 @@
     <t>THUMB NUT 1/4-20, PLASTIC HEAD</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00012</t>
+    <t>MECA-MECA-STD-COMPNT-AAAN</t>
   </si>
   <si>
     <t>93945K11</t>
@@ -3785,7 +3785,7 @@
     <t>DAMPING SANDWICH MOUNT WITH STUD AND INSERT, 1/4-20, NEOPRENE, 15 LB</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00013</t>
+    <t>MECA-MECA-STD-COMPNT-AAAP</t>
   </si>
   <si>
     <t>94052A133</t>
@@ -3794,7 +3794,7 @@
     <t>SCREW-HEAD MOUNT KNOB, KNURLED, ACETAL, FOR 1/4 SCREW, 3/4 OD, BLACK</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00014</t>
+    <t>MECA-MECA-STD-COMPNT-AAAQ</t>
   </si>
   <si>
     <t>9657K309</t>
@@ -3803,7 +3803,7 @@
     <t>RESSORT DE COMPRESSION, ID 0.39, OD 0.48, 1.0 LG, 12 LB</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00015</t>
+    <t>MECA-MECA-STD-COMPNT-AAAR</t>
   </si>
   <si>
     <t>97447A045</t>
@@ -3812,7 +3812,7 @@
     <t>RIVET ALUMINIUM 3/16, ÉP.1/16-1/8, PERCER NO.11</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00016</t>
+    <t>MECA-MECA-STD-COMPNT-AAAS</t>
   </si>
   <si>
     <t>97447A050</t>
@@ -3821,7 +3821,7 @@
     <t>RIVET ALUMINIUM 3/16, ÉP.1/8-1/4, PERCER NO.11</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00017</t>
+    <t>MECA-MECA-STD-COMPNT-AAAT</t>
   </si>
   <si>
     <t>97526A411</t>
@@ -3830,7 +3830,7 @@
     <t>RIVET ALUMINIUM NOIR 3/16" X 0.250"</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00018</t>
+    <t>MECA-MECA-STD-COMPNT-AAAW</t>
   </si>
   <si>
     <t>98296A916</t>
@@ -3839,7 +3839,7 @@
     <t>GOUPILLE FENDUE 3/16" X 1 3/4" LG.</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00019</t>
+    <t>MECA-MECA-STD-COMPNT-AAAX</t>
   </si>
   <si>
     <t>98381A714</t>
@@ -3848,7 +3848,7 @@
     <t>DOWEL PIN 1/2 X 1-1/4, 4037-4140 ALLOY</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00020</t>
+    <t>MECA-MECA-STD-COMPNT-AAAY</t>
   </si>
   <si>
     <t>99142A665</t>
@@ -3857,7 +3857,7 @@
     <t>ANNEAU DE RETENUE INTERNE DIAM. 3-1/4"</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00021</t>
+    <t>MECA-MECA-STD-COMPNT-AAAZ</t>
   </si>
   <si>
     <t>0801733</t>
@@ -3869,7 +3869,7 @@
     <t>PHOENIX CONTACT</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00022</t>
+    <t>MECA-MECA-STD-COMPNT-AAA2</t>
   </si>
   <si>
     <t>3240192</t>
@@ -3878,7 +3878,7 @@
     <t>GOULOTTE 40 X 60 MM</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00023</t>
+    <t>MECA-MECA-STD-COMPNT-AAA3</t>
   </si>
   <si>
     <t>3240263</t>
@@ -3887,7 +3887,7 @@
     <t>GOULOTTE PASSAGE DE FIL 60 MM X 100 MM</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00024</t>
+    <t>MECA-MECA-STD-COMPNT-AAA4</t>
   </si>
   <si>
     <t>CSR34</t>
@@ -3899,7 +3899,7 @@
     <t>RICHELIEU</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00025</t>
+    <t>MECA-MECA-STD-COMPNT-AAA5</t>
   </si>
   <si>
     <t>BEF-WNL01MPA</t>
@@ -3908,7 +3908,7 @@
     <t>BRACKET DE FIXATION HORIZONTAL POUR LECTEUR MAGNÉTIQUE MLS</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00026</t>
+    <t>MECA-MECA-STD-COMPNT-AAA6</t>
   </si>
   <si>
     <t>GEZ-200-ESX-2LS</t>
@@ -3920,7 +3920,7 @@
     <t>SKF</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00027</t>
+    <t>MECA-MECA-STD-COMPNT-AAA7</t>
   </si>
   <si>
     <t>ZMS58-S-H0-K01</t>
@@ -3929,7 +3929,7 @@
     <t>TORQUE SUPPORT FOR Ø58MM SERIES, SYNCHRONISER FLANGE, NO HEIGHT ADAPTER</t>
   </si>
   <si>
-    <t>MECA-MECA-COMP-018C-00028</t>
+    <t>MECA-MECA-STD-COMPNT-AAA8</t>
   </si>
   <si>
     <t>3005.2172.25</t>
@@ -3941,7 +3941,7 @@
     <t>EXTREME MAX</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00001</t>
+    <t>MECA-STD-BOLT-VISSER-AAAA</t>
   </si>
   <si>
     <t>90385A199</t>
@@ -3953,7 +3953,7 @@
     <t>015 | BOULONNERIE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00002</t>
+    <t>MECA-STD-BOLT-VISSER-AAAB</t>
   </si>
   <si>
     <t>90631A411</t>
@@ -3962,7 +3962,7 @@
     <t>ÉCROU AUTOBLOQUANT A GARNITURE EN NYLON #10-32</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00003</t>
+    <t>MECA-STD-BOLT-VISSER-AAAC</t>
   </si>
   <si>
     <t>92220A252</t>
@@ -3971,7 +3971,7 @@
     <t>LOW-PROFILE SHCS  3/8"-16 X 3/4" FULLY THREADED, BLACK OXYDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00004</t>
+    <t>MECA-STD-BOLT-VISSER-AAAD</t>
   </si>
   <si>
     <t>92316A536_</t>
@@ -3980,7 +3980,7 @@
     <t>FLANGED HEX CAP SCREW, GRADE 8, BLACK PHOSPHATE, 1/4-20 X 1/2"</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00005</t>
+    <t>MECA-STD-BOLT-VISSER-AAAE</t>
   </si>
   <si>
     <t>92316A540</t>
@@ -3989,7 +3989,7 @@
     <t>FLANGED HEX CAP SCREW, GRADE 8, BLACK PHOSPHATE, 1/4-20 X 3/4"</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00006</t>
+    <t>MECA-STD-BOLT-VISSER-AAAF</t>
   </si>
   <si>
     <t>92316A624</t>
@@ -3998,7 +3998,7 @@
     <t>FLANGED HEX CAP SCREW, GRADE 8, BLACK PHOSPHATE, 3/8-16 X 1"</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00007</t>
+    <t>MECA-STD-BOLT-VISSER-AAAG</t>
   </si>
   <si>
     <t>92785A333</t>
@@ -4007,7 +4007,7 @@
     <t>SET SCREW 10-32 X 5/16 LG., CONE POINT, SS 18-8</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00008</t>
+    <t>MECA-STD-BOLT-VISSER-AAAH</t>
   </si>
   <si>
     <t>93560A160</t>
@@ -4016,7 +4016,7 @@
     <t>STEEL HEX WELD NUT, 3/8-16, FOR HOLE 35/64"DIA.</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00009</t>
+    <t>MECA-STD-BOLT-VISSER-AAAJ</t>
   </si>
   <si>
     <t>94945A205_</t>
@@ -4025,7 +4025,7 @@
     <t>HIGH STRENGTH THIN HEX NUT, NYLON INSERT, 1/4-20</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00010</t>
+    <t>MECA-STD-BOLT-VISSER-AAAK</t>
   </si>
   <si>
     <t>96660A173</t>
@@ -4034,7 +4034,7 @@
     <t>FLANGED BUTTON 1/4-20 X 1" FULLY THREADED, ZINC-PLATED</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00011</t>
+    <t>MECA-STD-BOLT-VISSER-AAAM</t>
   </si>
   <si>
     <t>97131A110</t>
@@ -4043,7 +4043,7 @@
     <t>HEX NYLON LOCKNUT, M4, CLASS 8, ZINC PLATED</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00012</t>
+    <t>MECA-STD-BOLT-VISSER-AAAN</t>
   </si>
   <si>
     <t>97135A210_</t>
@@ -4052,7 +4052,7 @@
     <t>ÉCROU AUTOBLOQUANT À GARNITURE EN NYLON, GR. 8, CHROMATE PLATED, 1/4-20</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00013</t>
+    <t>MECA-STD-BOLT-VISSER-AAAP</t>
   </si>
   <si>
     <t>97135A220</t>
@@ -4061,7 +4061,7 @@
     <t>ÉCROU AUTOBLOQUANT À GARNITURE EN NYLON, GR. 8, CHROMATE PLATED, 5/16-18</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00014</t>
+    <t>MECA-STD-BOLT-VISSER-AAAQ</t>
   </si>
   <si>
     <t>99461A120</t>
@@ -4070,7 +4070,7 @@
     <t>THREAD-FORMING SCREW, TRI-LOBE, #4-20 X 3/8''LG</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00015</t>
+    <t>MECA-STD-BOLT-VISSER-AAAR</t>
   </si>
   <si>
     <t>99461A240</t>
@@ -4079,7 +4079,7 @@
     <t>THREAD-FORMING SCREW, TRI-LOBE, #6-19 X 1/2''LG</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00016</t>
+    <t>MECA-STD-BOLT-VISSER-AAAS</t>
   </si>
   <si>
     <t>FSHCS 0.25-20x0.5x0.5-HX-BO</t>
@@ -4091,7 +4091,7 @@
     <t>ND</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00017</t>
+    <t>MECA-STD-BOLT-VISSER-AAAT</t>
   </si>
   <si>
     <t>FSHCS 0.25-20x0.75x0.75-HX-BO</t>
@@ -4100,7 +4100,7 @@
     <t>FLAT SOCKET HEAD CAP HEAD SCREW 82°, 1/4-20 X 0.75'' LG, FULLY THREADED, GRADE 5, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00018</t>
+    <t>MECA-STD-BOLT-VISSER-AAAW</t>
   </si>
   <si>
     <t>FSHCS 0.25-20x1x1-HX-BO</t>
@@ -4109,7 +4109,7 @@
     <t>FLAT SOCKET HEAD CAP HEAD SCREW 82°, 1/4-20 X 1'' LG, FULLY THREADED, GRADE 5, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00019</t>
+    <t>MECA-STD-BOLT-VISSER-AAAX</t>
   </si>
   <si>
     <t>FSHCS M3x8x8-HX-BO</t>
@@ -4118,7 +4118,7 @@
     <t>FLAT SOCKET HEAD CAP SCREW 90°, M3 X 8MM LG, FULLY THREADED, CLASS 10.9, ISO 10642, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00020</t>
+    <t>MECA-STD-BOLT-VISSER-AAAY</t>
   </si>
   <si>
     <t>FSHCS M4x12x12-HX-BO</t>
@@ -4127,7 +4127,7 @@
     <t>FLAT SOCKET HEAD CAP SCREW 90°, M4 X 12MM LG, FULLY THREADED, CLASS 10.9, ISO 10642, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00021</t>
+    <t>MECA-STD-BOLT-VISSER-AAAZ</t>
   </si>
   <si>
     <t>FSHCS M4X12X12-ZP</t>
@@ -4136,7 +4136,7 @@
     <t>FLAT SOCKET HEAD CAP SCREW 90°, M4 X 12MM LG, FULLY THREADED, CLASS 10.9, ISO 10642, ZINC PLATED</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00022</t>
+    <t>MECA-STD-BOLT-VISSER-AAA2</t>
   </si>
   <si>
     <t>FW #10</t>
@@ -4145,7 +4145,7 @@
     <t>FLAT WASHER FOR BOLT #10, 0.219 X 0.5, ASME B18.21.1, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00023</t>
+    <t>MECA-STD-BOLT-VISSER-AAA3</t>
   </si>
   <si>
     <t>FW #6</t>
@@ -4154,7 +4154,7 @@
     <t>FLAT WASHER FOR BOLT #6, 0.156 X 0.375, ASME B18.21.1, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00024</t>
+    <t>MECA-STD-BOLT-VISSER-AAA4</t>
   </si>
   <si>
     <t>FW #8</t>
@@ -4163,7 +4163,7 @@
     <t>FLAT WASHER FOR BOLT #8, 0.188 X 0.438, ASME B18.21.1, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00025</t>
+    <t>MECA-STD-BOLT-VISSER-AAA5</t>
   </si>
   <si>
     <t>FW 0,25</t>
@@ -4172,7 +4172,7 @@
     <t>FLAT WASHER FOR BOLT 1/4, 0.281 X 0.625, ASME B18.21.1, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00026</t>
+    <t>MECA-STD-BOLT-VISSER-AAA6</t>
   </si>
   <si>
     <t>FW 0,3125</t>
@@ -4181,7 +4181,7 @@
     <t>FLAT WASHER FOR BOLT 5/16, 0.344 X 0.688, ASME B18.21.1, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00027</t>
+    <t>MECA-STD-BOLT-VISSER-AAA7</t>
   </si>
   <si>
     <t>FW 0,5</t>
@@ -4190,7 +4190,7 @@
     <t>FLAT WASHER FOR BOLT 1/2, 0.531 X 1.062, ASME B18.21.1, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00028</t>
+    <t>MECA-STD-BOLT-VISSER-AAA8</t>
   </si>
   <si>
     <t>FW M4</t>
@@ -4199,7 +4199,7 @@
     <t>FLAT WASHER FOR BOLT M4, ISO 7089, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00029</t>
+    <t>MECA-STD-BOLT-VISSER-AAA9</t>
   </si>
   <si>
     <t>FW M5</t>
@@ -4208,7 +4208,7 @@
     <t>FLAT WASHER FOR BOLT M5, ISO 7089, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00030</t>
+    <t>MECA-STD-BOLT-VISSER-AABA</t>
   </si>
   <si>
     <t>HHCS 0.5000-13x2.25x1.25-BO</t>
@@ -4217,7 +4217,7 @@
     <t>HEX HEAD CAP SCREW, 1/2-13 X 2.25'' LG, X 1.25'' THREAD LENGHT, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00031</t>
+    <t>MECA-STD-BOLT-VISSER-AABB</t>
   </si>
   <si>
     <t>HNUT M5-0.8-D-BO</t>
@@ -4226,7 +4226,7 @@
     <t>HEX NUT, M5, CLASS 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00032</t>
+    <t>MECA-STD-BOLT-VISSER-AABC</t>
   </si>
   <si>
     <t>HX-SHCS 0.25-20x0.5x0.5-N</t>
@@ -4235,7 +4235,7 @@
     <t>SOCKET HEAD CAP SCREW, 1/4-20 X 1/2'' LG, GRADE 8</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00033</t>
+    <t>MECA-STD-BOLT-VISSER-AABD</t>
   </si>
   <si>
     <t>HX-SHCS 0.25-20x1x1-N</t>
@@ -4244,7 +4244,7 @@
     <t>SOCKET HEAD CAP SCREW, 1/4-20 X 1'' LG, ASTM A574</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00034</t>
+    <t>MECA-STD-BOLT-VISSER-AABE</t>
   </si>
   <si>
     <t>LSHNUT 0.138-32-D-BO</t>
@@ -4253,7 +4253,7 @@
     <t>LOW STRENGHT HEX NUT, #6-32, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00035</t>
+    <t>MECA-STD-BOLT-VISSER-AABF</t>
   </si>
   <si>
     <t>LW 0.25</t>
@@ -4262,7 +4262,7 @@
     <t>SPLIT LOCK WASHER FOR BOLT 1/4, ASME B18.21.1</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00036</t>
+    <t>MECA-STD-BOLT-VISSER-AABG</t>
   </si>
   <si>
     <t>LW M10</t>
@@ -4271,7 +4271,7 @@
     <t>SPLIT LOCK WASHER FOR BOLT M10, DIN 127B</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00037</t>
+    <t>MECA-STD-BOLT-VISSER-AABH</t>
   </si>
   <si>
     <t>SBHCS 0.138-32x0.375-HX-BO</t>
@@ -4280,7 +4280,7 @@
     <t>HEX SOCKET BUTTON HEAD CAP SCREW, #6-32 X 0.375'' LG, FULLY THREADED, GRADE 5, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00038</t>
+    <t>MECA-STD-BOLT-VISSER-AABJ</t>
   </si>
   <si>
     <t>SBHCS 0.138-32x0.5-HX-BO</t>
@@ -4289,7 +4289,7 @@
     <t>HEX SOCKET BUTTON HEAD CAP SCREW, #6-32 X 0.5'' LG, FULLY THREADED, GRADE 5, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00039</t>
+    <t>MECA-STD-BOLT-VISSER-AABK</t>
   </si>
   <si>
     <t>SBHCS 0.25-20x0.375-HX-BO</t>
@@ -4298,7 +4298,7 @@
     <t>HEX SOCKET BUTTON HEAD CAP SCREW, 1/4-20 X 0.375'' LG, FULLY THREADED, GRADE 5, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00040</t>
+    <t>MECA-STD-BOLT-VISSER-AABM</t>
   </si>
   <si>
     <t>SBHCS 0.25-20x1-HX-BO</t>
@@ -4307,7 +4307,7 @@
     <t>HEX SOCKET BUTTON HEAD CAP SCREW, 1/4-20 X 1'' LG, FULLY THREADED, GRADE 5, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00041</t>
+    <t>MECA-STD-BOLT-VISSER-AABN</t>
   </si>
   <si>
     <t>SBHCS 0.3125-18x0.75-HX-BO</t>
@@ -4316,7 +4316,7 @@
     <t>HEX SOCKET BUTTON HEAD CAP SCREW, 5/16-18 X 0.75'' LG, FULLY THREADED, GRADE 5, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00042</t>
+    <t>MECA-STD-BOLT-VISSER-AABP</t>
   </si>
   <si>
     <t>SBHCS M3x10-HX-BO</t>
@@ -4325,7 +4325,7 @@
     <t>HEX SOCKET BUTTON HEAD CAP SCREW, M3 X 10MM LG, FULLY THREADED, CLASS 10.9, ISO 7380, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00043</t>
+    <t>MECA-STD-BOLT-VISSER-AABQ</t>
   </si>
   <si>
     <t>SBHCS M4x12-HX-BO</t>
@@ -4334,7 +4334,7 @@
     <t>HEX SOCKET BUTTON HEAD CAP SCREW, M4 X 12MM LG, FULLY THREADED, CLASS 10.9, ISO 7380, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00044</t>
+    <t>MECA-STD-BOLT-VISSER-AABR</t>
   </si>
   <si>
     <t>SHCS 0.138-32x0.25x0.25-HX-BO</t>
@@ -4343,7 +4343,7 @@
     <t>SOCKET HEAD CAP SCREW, #6-32 X 0.25'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00045</t>
+    <t>MECA-STD-BOLT-VISSER-AABS</t>
   </si>
   <si>
     <t>SHCS 0.138-32x0.375x0.375-HX-BO</t>
@@ -4352,7 +4352,7 @@
     <t>SOCKET HEAD CAP SCREW, #6-32 X 0.375'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00046</t>
+    <t>MECA-STD-BOLT-VISSER-AABT</t>
   </si>
   <si>
     <t>SHCS 0.138-40x0.875x0.875-HX-BO</t>
@@ -4361,7 +4361,7 @@
     <t>SOCKET HEAD CAP SCREW, #6-40 X 0.875'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00047</t>
+    <t>MECA-STD-BOLT-VISSER-AABW</t>
   </si>
   <si>
     <t>SHCS 0.164-32x0.3125x0.3125-HX-BO</t>
@@ -4370,7 +4370,7 @@
     <t>SOCKET HEAD CAP SCREW, #8-32 X 0.3125'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00048</t>
+    <t>MECA-STD-BOLT-VISSER-AABX</t>
   </si>
   <si>
     <t>SHCS 0.164-32x0.375x0.375-HX-BO</t>
@@ -4379,7 +4379,7 @@
     <t>SOCKET HEAD CAP SCREW, #8-32 X 0.375'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00049</t>
+    <t>MECA-STD-BOLT-VISSER-AABY</t>
   </si>
   <si>
     <t>SHCS 0.164-32x0.5x0.5-HX-BO</t>
@@ -4388,7 +4388,7 @@
     <t>SOCKET HEAD CAP SCREW, #8-32 X 0.5'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00050</t>
+    <t>MECA-STD-BOLT-VISSER-AABZ</t>
   </si>
   <si>
     <t>SHCS 0.164-32x0.625x0.625-HX-BO</t>
@@ -4397,7 +4397,7 @@
     <t>SOCKET HEAD CAP SCREW, #8-32 X 0.625'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00051</t>
+    <t>MECA-STD-BOLT-VISSER-AAB2</t>
   </si>
   <si>
     <t>SHCS 0.164-32x0.75x0.75-HX-BO</t>
@@ -4406,7 +4406,7 @@
     <t>SOCKET HEAD CAP SCREW, #8-32 X 0.75'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00052</t>
+    <t>MECA-STD-BOLT-VISSER-AAB3</t>
   </si>
   <si>
     <t>SHCS 0.164-32x1.125x1.125-HX-BO</t>
@@ -4415,7 +4415,7 @@
     <t>SOCKET HEAD CAP SCREW, #8-32 X 1.125'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00053</t>
+    <t>MECA-STD-BOLT-VISSER-AAB4</t>
   </si>
   <si>
     <t>SHCS 0.19-32x0.25x0.25-HX-BO</t>
@@ -4424,7 +4424,7 @@
     <t>SOCKET HEAD CAP SCREW, #10-32 X 0.25'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00054</t>
+    <t>MECA-STD-BOLT-VISSER-AAB5</t>
   </si>
   <si>
     <t>SHCS 0.19-32x0.3125x0.3125-HX-BO</t>
@@ -4433,7 +4433,7 @@
     <t>SOCKET HEAD CAP SCREW, #10-32 X 0.3125'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00055</t>
+    <t>MECA-STD-BOLT-VISSER-AAB6</t>
   </si>
   <si>
     <t>SHCS 0.19-32x0.375x0.375-HX-BO</t>
@@ -4442,7 +4442,7 @@
     <t>SOCKET HEAD CAP SCREW, #10-32 X 0.375'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00056</t>
+    <t>MECA-STD-BOLT-VISSER-AAB7</t>
   </si>
   <si>
     <t>SHCS 0.19-32x0.375x0.375-HX-N</t>
@@ -4451,7 +4451,7 @@
     <t>HEX SOCKET HEAD CAP SCREW, #10-32 X 0.375'' LG, FULLY THREADED, GRADE 8</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00057</t>
+    <t>MECA-STD-BOLT-VISSER-AAB8</t>
   </si>
   <si>
     <t>SHCS 0.19-32x0.625x0.625-HX-BO</t>
@@ -4460,7 +4460,7 @@
     <t>SOCKET HEAD CAP SCREW, #10-32 X 0.625'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00058</t>
+    <t>MECA-STD-BOLT-VISSER-AAB9</t>
   </si>
   <si>
     <t>SHCS 0.19-32x1.625x1.25-HX-BO</t>
@@ -4469,7 +4469,7 @@
     <t>SOCKET HEAD CAP SCREW, #10-32 X 1.625'' LG, X 1.25'' THREAD LENGHT, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00059</t>
+    <t>MECA-STD-BOLT-VISSER-AACA</t>
   </si>
   <si>
     <t>SHCS 0.25-20x0.375x0.375-HX-BO</t>
@@ -4478,7 +4478,7 @@
     <t>SOCKET HEAD CAP SCREW, 1/4-20 X 0.375'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00060</t>
+    <t>MECA-STD-BOLT-VISSER-AACB</t>
   </si>
   <si>
     <t>SHCS 0.25-20x0.5x0.5-HX-BO</t>
@@ -4487,7 +4487,7 @@
     <t>SOCKET HEAD CAP SCREW, 1/4-20 X 0.5'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00061</t>
+    <t>MECA-STD-BOLT-VISSER-AACC</t>
   </si>
   <si>
     <t>SHCS 0.25-20x0.75x0.75-HX-BO</t>
@@ -4496,7 +4496,7 @@
     <t>SOCKET HEAD CAP SCREW, 1/4-20 X 0.75'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00062</t>
+    <t>MECA-STD-BOLT-VISSER-AACD</t>
   </si>
   <si>
     <t>SHCS 0.25-20x0.875x0.875-HX-BO</t>
@@ -4505,7 +4505,7 @@
     <t>SOCKET HEAD CAP SCREW, 1/4-20 X 0.875'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00063</t>
+    <t>MECA-STD-BOLT-VISSER-AACE</t>
   </si>
   <si>
     <t>SHCS 0.25-20x1.5x1.5-HX-BO</t>
@@ -4514,7 +4514,7 @@
     <t>SOCKET HEAD CAP SCREW, 1/4-20 X 1.5'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00064</t>
+    <t>MECA-STD-BOLT-VISSER-AACF</t>
   </si>
   <si>
     <t>SHCS 0.25-20x1x1-HX-BO</t>
@@ -4523,7 +4523,7 @@
     <t>SOCKET HEAD CAP SCREW, 1/4-20 X 1'' LG, FULLY THREADED, GRADE 8, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00065</t>
+    <t>MECA-STD-BOLT-VISSER-AACG</t>
   </si>
   <si>
     <t>SHCS M10x40x40HX-N</t>
@@ -4532,7 +4532,7 @@
     <t>HEX SOCKET HEAD CAP SCREW, M10 X 40MM LG, FULLY THREADED, CLASS 12.9, ISO 4762</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00066</t>
+    <t>MECA-STD-BOLT-VISSER-AACH</t>
   </si>
   <si>
     <t>SHCS M4x16x16HX-BO</t>
@@ -4541,7 +4541,7 @@
     <t>HEX SOCKET HEAD CAP SCREW, M4 X 16MM LG, FULLY THREADED, CLASS 12.9, ISO 4762, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00067</t>
+    <t>MECA-STD-BOLT-VISSER-AACJ</t>
   </si>
   <si>
     <t>SHCS M4x6x6HX-BO</t>
@@ -4550,7 +4550,7 @@
     <t>HEX SOCKET HEAD CAP SCREW, M4 X 6MM LG, FULLY THREADED, CLASS 12.9, ISO 4762, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00068</t>
+    <t>MECA-STD-BOLT-VISSER-AACK</t>
   </si>
   <si>
     <t>SHCS M5x12x12HX-BO</t>
@@ -4559,7 +4559,7 @@
     <t>HEX SOCKET HEAD CAP SCREW, M5 X 12MM LG, FULLY THREADED, CLASS 12.9, ISO 4762, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00069</t>
+    <t>MECA-STD-BOLT-VISSER-AACM</t>
   </si>
   <si>
     <t>SHCS M5x40x22HX-BO</t>
@@ -4568,7 +4568,7 @@
     <t>HEX SOCKET HEAD CAP SCREW, M5 X 40MM LG, X 22MM THREAD LENGHT, CLASS 12.9, ISO 4762, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00070</t>
+    <t>MECA-STD-BOLT-VISSER-AACN</t>
   </si>
   <si>
     <t>SHCS M6x22x22HX-BO</t>
@@ -4577,7 +4577,7 @@
     <t>HEX SOCKET HEAD CAP SCREW, M6 X 22MM LG, FULLY THREADED, CLASS 12.9, ISO 4762, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-BOLT-BOLT-015B-00071</t>
+    <t>MECA-STD-BOLT-VISSER-AACP</t>
   </si>
   <si>
     <t>SHCS M8x25x25HX-BO</t>
@@ -4586,7 +4586,7 @@
     <t>HEX SOCKET HEAD CAP SCREW, M8 X 25MM LG, FULLY THREADED, CLASS 12.9, ISO 4762, BLACK OXIDE</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00001</t>
+    <t>MECA-STD-POLY-PLASTI-AAAA</t>
   </si>
   <si>
     <t>D-0050322</t>
@@ -4598,7 +4598,7 @@
     <t>004 | PLASTIQUE (UHMW, LEXAN, ...)</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00002</t>
+    <t>MECA-STD-POLY-PLASTI-AAAB</t>
   </si>
   <si>
     <t>D-0050325</t>
@@ -4607,7 +4607,7 @@
     <t>CARROSSERIE PL - CÔTÉ BAS - LG 6</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00003</t>
+    <t>MECA-STD-POLY-PLASTI-AAAC</t>
   </si>
   <si>
     <t>D-0050328</t>
@@ -4616,7 +4616,7 @@
     <t>CARROSSERIE PL - CÔTÉ BAS - LG 4</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00004</t>
+    <t>MECA-STD-POLY-PLASTI-AAAD</t>
   </si>
   <si>
     <t>D-0050447</t>
@@ -4625,7 +4625,7 @@
     <t>CARROSSERIE PL - COIN BAS SANS BALAYEUR</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00005</t>
+    <t>MECA-STD-POLY-PLASTI-AAAE</t>
   </si>
   <si>
     <t>D-0054457</t>
@@ -4634,7 +4634,7 @@
     <t>CARROSSERIE PL4x - ARRIÈRE HAUT A</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00006</t>
+    <t>MECA-STD-POLY-PLASTI-AAAF</t>
   </si>
   <si>
     <t>D-0054458</t>
@@ -4643,7 +4643,7 @@
     <t>CARROSSERIE PL4x - ARRIÈRE HAUT B</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00007</t>
+    <t>MECA-STD-POLY-PLASTI-AAAG</t>
   </si>
   <si>
     <t>D-0054460</t>
@@ -4652,7 +4652,7 @@
     <t>CARROSSERIE PL4x - AVANT HAUT A</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00008</t>
+    <t>MECA-STD-POLY-PLASTI-AAAH</t>
   </si>
   <si>
     <t>D-0054461</t>
@@ -4661,7 +4661,7 @@
     <t>CARROSSERIE PL4x - AVANT HAUT B</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00009</t>
+    <t>MECA-STD-POLY-PLASTI-AAAJ</t>
   </si>
   <si>
     <t>D-0054462</t>
@@ -4670,7 +4670,7 @@
     <t>CARROSSERIE PL - COIN HAUT A</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00010</t>
+    <t>MECA-STD-POLY-PLASTI-AAAK</t>
   </si>
   <si>
     <t>D-0054463</t>
@@ -4679,7 +4679,7 @@
     <t>CARROSSERIE PL - COIN HAUT B</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00011</t>
+    <t>MECA-STD-POLY-PLASTI-AAAM</t>
   </si>
   <si>
     <t>D-0054464</t>
@@ -4688,7 +4688,7 @@
     <t>CARROSSERIE PLx6 - CÔTÉ HAUT A</t>
   </si>
   <si>
-    <t>MECA-PLAST-POLY-004P-00012</t>
+    <t>MECA-STD-POLY-PLASTI-AAAN</t>
   </si>
   <si>
     <t>D-0054465</t>
@@ -4697,13 +4697,13 @@
     <t>CARROSSERIE PLx6 - CÔTÉ HAUT B</t>
   </si>
   <si>
-    <t>MECA-MECA-STD-VIDE-00001</t>
+    <t>MECA-MECA-STD-VIDE-AAAA</t>
   </si>
   <si>
     <t>(vide)</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00001</t>
+    <t>MECA-ASS-STD-MONTER-AAAA</t>
   </si>
   <si>
     <t>A-0008889</t>
@@ -4715,7 +4715,7 @@
     <t>101 | ASSEMBLAGE MÉCANIQUE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00002</t>
+    <t>MECA-ASS-STD-MONTER-AAAB</t>
   </si>
   <si>
     <t>A-0008929</t>
@@ -4724,7 +4724,7 @@
     <t>MODULE DE BATTERIE ET RECHARGE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00003</t>
+    <t>MECA-ASS-STD-MONTER-AAAC</t>
   </si>
   <si>
     <t>A-0008956</t>
@@ -4733,7 +4733,7 @@
     <t>SUSPENSION ARRIÈRE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00004</t>
+    <t>MECA-ASS-STD-MONTER-AAAD</t>
   </si>
   <si>
     <t>A-0009798</t>
@@ -4742,7 +4742,7 @@
     <t>SUSPENSION GAUCHE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00005</t>
+    <t>MECA-ASS-STD-MONTER-AAAE</t>
   </si>
   <si>
     <t>A-0009799</t>
@@ -4751,7 +4751,7 @@
     <t>SUSPENSION DROITE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00006</t>
+    <t>MECA-ASS-STD-MONTER-AAAF</t>
   </si>
   <si>
     <t>A-0009811</t>
@@ -4760,7 +4760,7 @@
     <t>CARROSSERIE PL4x - PANNEAU AVANT</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00007</t>
+    <t>MECA-ASS-STD-MONTER-AAAG</t>
   </si>
   <si>
     <t>A-0009812</t>
@@ -4769,7 +4769,7 @@
     <t>CARROSSERIE PL4x - PANNEAU ARRIÈRE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00008</t>
+    <t>MECA-ASS-STD-MONTER-AAAH</t>
   </si>
   <si>
     <t>A-0009814</t>
@@ -4778,7 +4778,7 @@
     <t>CARROSSERIE PLx6 - PANNEAU CÔTÉS</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00009</t>
+    <t>MECA-ASS-STD-MONTER-AAAJ</t>
   </si>
   <si>
     <t>A-0009816</t>
@@ -4787,13 +4787,13 @@
     <t>CARROSSERIE PL - PANNEAU COIN HAUT</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00010</t>
+    <t>MECA-ASS-STD-MONTER-AAAK</t>
   </si>
   <si>
     <t>A-0009832</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00011</t>
+    <t>MECA-ASS-STD-MONTER-AAAM</t>
   </si>
   <si>
     <t>A-0009835</t>
@@ -4802,7 +4802,7 @@
     <t>SUPPORT D'AJUSTEMENT BALAYEUR LASER</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00012</t>
+    <t>MECA-ASS-STD-MONTER-AAAN</t>
   </si>
   <si>
     <t>A-0009844</t>
@@ -4811,7 +4811,7 @@
     <t>S-ASS PLAQUE ÉLECTRIQUE ARRIÈRE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00013</t>
+    <t>MECA-ASS-STD-MONTER-AAAP</t>
   </si>
   <si>
     <t>A-0009845</t>
@@ -4820,7 +4820,7 @@
     <t>ASSEMBLAGE PASSE PAROI - BATTERIE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00014</t>
+    <t>MECA-ASS-STD-MONTER-AAAQ</t>
   </si>
   <si>
     <t>A-0009846</t>
@@ -4829,7 +4829,7 @@
     <t>ASS. CONNECTEURS PASSE PAROI - MOTEUR CENTRE DROIT</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00015</t>
+    <t>MECA-ASS-STD-MONTER-AAAR</t>
   </si>
   <si>
     <t>A-0009847</t>
@@ -4838,7 +4838,7 @@
     <t>ASS. CONNECTEURs PASSE PAROI - MOTEUR CÔTÉ</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00016</t>
+    <t>MECA-ASS-STD-MONTER-AAAS</t>
   </si>
   <si>
     <t>A-0009848</t>
@@ -4847,7 +4847,7 @@
     <t>ASSEMBLAGE DIAGNOSTIQUE ÉLECTRIQUE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00017</t>
+    <t>MECA-ASS-STD-MONTER-AAAT</t>
   </si>
   <si>
     <t>A-0009849</t>
@@ -4856,7 +4856,7 @@
     <t>ASS. CONNECTEUR PASSE PAROI - CÔTÉ EXT. AV.</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00018</t>
+    <t>MECA-ASS-STD-MONTER-AAAW</t>
   </si>
   <si>
     <t>A-0009850</t>
@@ -4865,7 +4865,7 @@
     <t>ASSEMBLAGE PASSE PAROI - CÔTÉ EXT. ARR.</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00019</t>
+    <t>MECA-ASS-STD-MONTER-AAAX</t>
   </si>
   <si>
     <t>A-0009851</t>
@@ -4874,7 +4874,7 @@
     <t>ASSEMBLAGE PASSE PAROI - AVANT INT. GAUCHE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00020</t>
+    <t>MECA-ASS-STD-MONTER-AAAY</t>
   </si>
   <si>
     <t>A-0009852</t>
@@ -4883,7 +4883,7 @@
     <t>ASSEMBLAGE PASSE PAROI - AVANT INT. DROIT</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00021</t>
+    <t>MECA-ASS-STD-MONTER-AAAZ</t>
   </si>
   <si>
     <t>A-0009853</t>
@@ -4892,7 +4892,7 @@
     <t>PRÉMONTAGE RFID</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00022</t>
+    <t>MECA-ASS-STD-MONTER-AAA2</t>
   </si>
   <si>
     <t>A-0009984</t>
@@ -4901,7 +4901,7 @@
     <t>ASSEMBLAGE SECTIONNEUR</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00023</t>
+    <t>MECA-ASS-STD-MONTER-AAA3</t>
   </si>
   <si>
     <t>A-0009997</t>
@@ -4910,7 +4910,7 @@
     <t>BOITIER ÉLECTRIQUE AGV PL</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00024</t>
+    <t>MECA-ASS-STD-MONTER-AAA4</t>
   </si>
   <si>
     <t>A-0009998</t>
@@ -4919,7 +4919,7 @@
     <t>ASSEMBLAGE DU BOÎTIER ÉLECTRIQUE PL.</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00025</t>
+    <t>MECA-ASS-STD-MONTER-AAA5</t>
   </si>
   <si>
     <t>A-0009999</t>
@@ -4928,7 +4928,7 @@
     <t>ASS. CONNECTEURS PASSE PAROI - MOTEUR CENTRE GAUCHE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00026</t>
+    <t>MECA-ASS-STD-MONTER-AAA6</t>
   </si>
   <si>
     <t>A-0010003</t>
@@ -4937,7 +4937,7 @@
     <t>ASSEMBLAGE PASSE-PAROI POUR 4X PP75</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00027</t>
+    <t>MECA-ASS-STD-MONTER-AAA7</t>
   </si>
   <si>
     <t>A-0010039</t>
@@ -4946,7 +4946,7 @@
     <t>PRÉMONTAGE ÉLECTRIQUE BATTERIE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00028</t>
+    <t>MECA-ASS-STD-MONTER-AAA8</t>
   </si>
   <si>
     <t>A-0010050</t>
@@ -4955,7 +4955,7 @@
     <t>ASSEMBLAGE RIVETÉ POUR COMPOSANTS BATTERIE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00029</t>
+    <t>MECA-ASS-STD-MONTER-AAA9</t>
   </si>
   <si>
     <t>A-0010072</t>
@@ -4964,7 +4964,7 @@
     <t>AMR-PL-4650-24L02#### COMPLET</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00030</t>
+    <t>MECA-ASS-STD-MONTER-AABA</t>
   </si>
   <si>
     <t>A-0010291</t>
@@ -4973,7 +4973,7 @@
     <t>S-ASS. LECTEUR MAGNÉTIQUE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00031</t>
+    <t>MECA-ASS-STD-MONTER-AABB</t>
   </si>
   <si>
     <t>A-0010507</t>
@@ -4982,7 +4982,7 @@
     <t>BOITIER DEL DEUTSCH ET RAIL DIN VERTICAL</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00032</t>
+    <t>MECA-ASS-STD-MONTER-AABC</t>
   </si>
   <si>
     <t>A-0010606</t>
@@ -4991,7 +4991,7 @@
     <t>CAROSSERIE PL46-ASS. COMPLET</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00033</t>
+    <t>MECA-ASS-STD-MONTER-AABD</t>
   </si>
   <si>
     <t>A-0010608</t>
@@ -5000,7 +5000,7 @@
     <t>ASSEMBLAGE ÉLECTRIQUE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00034</t>
+    <t>MECA-ASS-STD-MONTER-AABE</t>
   </si>
   <si>
     <t>A-0010609</t>
@@ -5009,7 +5009,7 @@
     <t>ASSEMBLAGE DES SUSPENSIONS</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-101S-00035</t>
+    <t>MECA-ASS-STD-MONTER-AABF</t>
   </si>
   <si>
     <t>A-0010610</t>
@@ -5018,7 +5018,7 @@
     <t>TOP ASS'Y</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-102S-00001</t>
+    <t>MECA-ASS-STD-322SSM-AAAA</t>
   </si>
   <si>
     <t>A-0008969</t>
@@ -5030,7 +5030,7 @@
     <t>102 | ASSEMBLAGE SOUDÉ</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-102S-00002</t>
+    <t>MECA-ASS-STD-322SSM-AAAB</t>
   </si>
   <si>
     <t>A-0008980</t>
@@ -5039,7 +5039,7 @@
     <t>BRAS DE SUSPENSION ARRIÈRE - CORPS SOUDÉ</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-102S-00003</t>
+    <t>MECA-ASS-STD-322SSM-AAAC</t>
   </si>
   <si>
     <t>A-0008991</t>
@@ -5048,7 +5048,7 @@
     <t>RENFORT INTERNE - AVANT</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-102S-00004</t>
+    <t>MECA-ASS-STD-322SSM-AAAD</t>
   </si>
   <si>
     <t>A-0008992</t>
@@ -5057,7 +5057,7 @@
     <t>RENFORT INTERNE - ARRIÈRE</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-102S-00005</t>
+    <t>MECA-ASS-STD-322SSM-AAAE</t>
   </si>
   <si>
     <t>A-0009071</t>
@@ -5066,7 +5066,7 @@
     <t>COMPOARTIMENT BATTERIES - ASS. SOUDÉ</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-102S-00006</t>
+    <t>MECA-ASS-STD-322SSM-AAAF</t>
   </si>
   <si>
     <t>A-0009801</t>
@@ -5075,7 +5075,7 @@
     <t>CHÂSSIS V2 - CORPS SOUDÉ</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-102S-00007</t>
+    <t>MECA-ASS-STD-322SSM-AAAG</t>
   </si>
   <si>
     <t>A-0009837</t>
@@ -5084,7 +5084,7 @@
     <t>RENFORT EXTÉRIEUR CÔTÉ</t>
   </si>
   <si>
-    <t>MECA-ASS-ASM-102S-00008</t>
+    <t>MECA-ASS-STD-322SSM-AAAH</t>
   </si>
   <si>
     <t>A-0009860</t>
@@ -5455,13 +5455,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="186.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
@@ -10643,13 +10643,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="B265" sqref="B265"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="98" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Add interactive component validation feature
Introduces a new validation window allowing users to select which BOM components will receive a SKU before generation. Updates documentation, adds tests and demo scripts, and refactors the interface for clarity and usability. The interface now displays SKU previews directly in the main table, removes redundant panels, and provides real-time statistics and feedback. Related files and tests have been added or updated to support this workflow.
</commit_message>
<xml_diff>
--- a/SKU_(V2.1) BOM unifié électrique-mécanique.xlsx
+++ b/SKU_(V2.1) BOM unifié électrique-mécanique.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcasaubon.NOOVELIA\OneDrive - Noovelia\Documents\GitHub\SKU-Generetor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://noovelia-my.sharepoint.com/personal/vcasaubon_noovelia_com/Documents/Documents/GitHub/SKU-Generetor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60218C7A-5EC4-48D2-AE3C-AFD92C922F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_47820CEC1A44987521BB2695395BDA1626CB0284" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{655F6C14-030A-440F-A80F-59581C81334C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="1690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="1688">
   <si>
     <t>SKU</t>
   </si>
@@ -2276,7 +2276,7 @@
     <t>K4</t>
   </si>
   <si>
-    <t>ELEC-ELEC-STD-RESIST-AAAA</t>
+    <t>ELEC-ELEC-STD-RESIST-AAAB</t>
   </si>
   <si>
     <t>RNMF14FTC120R</t>
@@ -4695,12 +4695,6 @@
   </si>
   <si>
     <t>CARROSSERIE PLx6 - CÔTÉ HAUT B</t>
-  </si>
-  <si>
-    <t>MECA-MECA-STD-VIDE-AAAA</t>
-  </si>
-  <si>
-    <t>(vide)</t>
   </si>
   <si>
     <t>MECA-ASS-STD-MONTER-AAAA</t>
@@ -5109,6 +5103,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5456,7 +5451,7 @@
   <dimension ref="A1:I178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10641,10 +10636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H279"/>
+  <dimension ref="A1:H278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16777,42 +16772,45 @@
         <v>1559</v>
       </c>
       <c r="C236" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D236" t="s">
-        <v>1559</v>
+        <v>1561</v>
       </c>
       <c r="E236" t="s">
-        <v>1559</v>
+        <v>832</v>
       </c>
       <c r="F236" t="s">
         <v>1559</v>
       </c>
+      <c r="G236">
+        <v>3</v>
+      </c>
       <c r="H236" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>1560</v>
+        <v>1562</v>
       </c>
       <c r="B237" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C237" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D237" t="s">
         <v>1561</v>
-      </c>
-      <c r="C237" t="s">
-        <v>1562</v>
-      </c>
-      <c r="D237" t="s">
-        <v>1563</v>
       </c>
       <c r="E237" t="s">
         <v>832</v>
       </c>
       <c r="F237" t="s">
-        <v>1561</v>
+        <v>1563</v>
       </c>
       <c r="G237">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H237" t="s">
         <v>833</v>
@@ -16820,22 +16818,22 @@
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="B238" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="C238" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D238" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E238" t="s">
         <v>832</v>
       </c>
       <c r="F238" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="G238">
         <v>1</v>
@@ -16846,22 +16844,22 @@
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="B239" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="C239" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D239" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E239" t="s">
         <v>832</v>
       </c>
       <c r="F239" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="G239">
         <v>1</v>
@@ -16872,22 +16870,22 @@
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="B240" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="C240" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D240" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E240" t="s">
         <v>832</v>
       </c>
       <c r="F240" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="G240">
         <v>1</v>
@@ -16898,22 +16896,22 @@
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="B241" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="C241" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D241" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E241" t="s">
         <v>832</v>
       </c>
       <c r="F241" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="G241">
         <v>1</v>
@@ -16924,22 +16922,22 @@
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="B242" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="C242" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D242" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E242" t="s">
         <v>832</v>
       </c>
       <c r="F242" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="G242">
         <v>1</v>
@@ -16950,25 +16948,25 @@
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="B243" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="C243" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D243" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E243" t="s">
         <v>832</v>
       </c>
       <c r="F243" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="G243">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H243" t="s">
         <v>833</v>
@@ -16976,25 +16974,25 @@
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="B244" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="C244" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D244" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E244" t="s">
         <v>832</v>
       </c>
       <c r="F244" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="G244">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H244" t="s">
         <v>833</v>
@@ -17002,25 +17000,25 @@
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="B245" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="C245" t="s">
-        <v>1587</v>
+        <v>990</v>
       </c>
       <c r="D245" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E245" t="s">
         <v>832</v>
       </c>
       <c r="F245" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="G245">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H245" t="s">
         <v>833</v>
@@ -17034,10 +17032,10 @@
         <v>1589</v>
       </c>
       <c r="C246" t="s">
-        <v>990</v>
+        <v>1590</v>
       </c>
       <c r="D246" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E246" t="s">
         <v>832</v>
@@ -17054,25 +17052,25 @@
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="B247" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="C247" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D247" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E247" t="s">
         <v>832</v>
       </c>
       <c r="F247" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="G247">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H247" t="s">
         <v>833</v>
@@ -17080,22 +17078,22 @@
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="B248" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="C248" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D248" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E248" t="s">
         <v>832</v>
       </c>
       <c r="F248" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="G248">
         <v>1</v>
@@ -17106,22 +17104,22 @@
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="B249" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="C249" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D249" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E249" t="s">
         <v>832</v>
       </c>
       <c r="F249" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="G249">
         <v>1</v>
@@ -17132,25 +17130,25 @@
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="B250" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="C250" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="D250" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E250" t="s">
         <v>832</v>
       </c>
       <c r="F250" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="G250">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H250" t="s">
         <v>833</v>
@@ -17158,25 +17156,25 @@
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="B251" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="C251" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="D251" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E251" t="s">
         <v>832</v>
       </c>
       <c r="F251" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="G251">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H251" t="s">
         <v>833</v>
@@ -17184,25 +17182,25 @@
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="B252" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="C252" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="D252" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E252" t="s">
         <v>832</v>
       </c>
       <c r="F252" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="G252">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H252" t="s">
         <v>833</v>
@@ -17210,22 +17208,22 @@
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="B253" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="C253" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="D253" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E253" t="s">
         <v>832</v>
       </c>
       <c r="F253" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="G253">
         <v>2</v>
@@ -17236,25 +17234,25 @@
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="B254" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="C254" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="D254" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E254" t="s">
         <v>832</v>
       </c>
       <c r="F254" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="G254">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H254" t="s">
         <v>833</v>
@@ -17262,22 +17260,22 @@
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="B255" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="C255" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="D255" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E255" t="s">
         <v>832</v>
       </c>
       <c r="F255" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="G255">
         <v>1</v>
@@ -17288,25 +17286,25 @@
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="B256" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="C256" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="D256" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E256" t="s">
         <v>832</v>
       </c>
       <c r="F256" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="G256">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H256" t="s">
         <v>833</v>
@@ -17314,25 +17312,25 @@
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="B257" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="C257" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="D257" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E257" t="s">
         <v>832</v>
       </c>
       <c r="F257" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="G257">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H257" t="s">
         <v>833</v>
@@ -17340,22 +17338,22 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="B258" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="C258" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="D258" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E258" t="s">
         <v>832</v>
       </c>
       <c r="F258" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="G258">
         <v>1</v>
@@ -17366,22 +17364,22 @@
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="B259" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="C259" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="D259" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E259" t="s">
         <v>832</v>
       </c>
       <c r="F259" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="G259">
         <v>1</v>
@@ -17392,22 +17390,22 @@
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="B260" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="C260" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="D260" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E260" t="s">
         <v>832</v>
       </c>
       <c r="F260" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="G260">
         <v>1</v>
@@ -17418,22 +17416,22 @@
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="B261" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="C261" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="D261" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E261" t="s">
         <v>832</v>
       </c>
       <c r="F261" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="G261">
         <v>1</v>
@@ -17444,22 +17442,22 @@
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="B262" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="C262" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="D262" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E262" t="s">
         <v>832</v>
       </c>
       <c r="F262" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="G262">
         <v>1</v>
@@ -17470,22 +17468,22 @@
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="B263" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="C263" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="D263" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E263" t="s">
         <v>832</v>
       </c>
       <c r="F263" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="G263">
         <v>1</v>
@@ -17496,22 +17494,22 @@
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="B264" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="C264" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="D264" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E264" t="s">
         <v>832</v>
       </c>
       <c r="F264" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="G264">
         <v>1</v>
@@ -17522,25 +17520,25 @@
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="B265" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="C265" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="D265" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E265" t="s">
         <v>832</v>
       </c>
       <c r="F265" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="G265">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H265" t="s">
         <v>833</v>
@@ -17548,25 +17546,25 @@
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="B266" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="C266" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="D266" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E266" t="s">
         <v>832</v>
       </c>
       <c r="F266" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="G266">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H266" t="s">
         <v>833</v>
@@ -17574,22 +17572,22 @@
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="B267" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="C267" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="D267" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E267" t="s">
         <v>832</v>
       </c>
       <c r="F267" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="G267">
         <v>1</v>
@@ -17600,22 +17598,22 @@
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="B268" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="C268" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="D268" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E268" t="s">
         <v>832</v>
       </c>
       <c r="F268" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="G268">
         <v>1</v>
@@ -17626,22 +17624,22 @@
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="B269" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="C269" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="D269" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E269" t="s">
         <v>832</v>
       </c>
       <c r="F269" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="G269">
         <v>1</v>
@@ -17652,22 +17650,22 @@
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="B270" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="C270" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="D270" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E270" t="s">
         <v>832</v>
       </c>
       <c r="F270" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="G270">
         <v>1</v>
@@ -17678,22 +17676,22 @@
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="B271" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="C271" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="D271" t="s">
-        <v>1563</v>
+        <v>1666</v>
       </c>
       <c r="E271" t="s">
         <v>832</v>
       </c>
       <c r="F271" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="G271">
         <v>1</v>
@@ -17704,22 +17702,22 @@
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>1665</v>
+        <v>1667</v>
       </c>
       <c r="B272" t="s">
+        <v>1668</v>
+      </c>
+      <c r="C272" t="s">
+        <v>1669</v>
+      </c>
+      <c r="D272" t="s">
         <v>1666</v>
-      </c>
-      <c r="C272" t="s">
-        <v>1667</v>
-      </c>
-      <c r="D272" t="s">
-        <v>1668</v>
       </c>
       <c r="E272" t="s">
         <v>832</v>
       </c>
       <c r="F272" t="s">
-        <v>1666</v>
+        <v>1668</v>
       </c>
       <c r="G272">
         <v>1</v>
@@ -17730,22 +17728,22 @@
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="B273" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="C273" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="D273" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="E273" t="s">
         <v>832</v>
       </c>
       <c r="F273" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="G273">
         <v>1</v>
@@ -17756,22 +17754,22 @@
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="B274" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="C274" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="D274" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="E274" t="s">
         <v>832</v>
       </c>
       <c r="F274" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="G274">
         <v>1</v>
@@ -17782,22 +17780,22 @@
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="B275" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="C275" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="D275" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="E275" t="s">
         <v>832</v>
       </c>
       <c r="F275" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="G275">
         <v>1</v>
@@ -17808,22 +17806,22 @@
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="B276" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="C276" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="D276" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="E276" t="s">
         <v>832</v>
       </c>
       <c r="F276" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="G276">
         <v>1</v>
@@ -17834,25 +17832,25 @@
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="B277" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="C277" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="D277" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="E277" t="s">
         <v>832</v>
       </c>
       <c r="F277" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="G277">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H277" t="s">
         <v>833</v>
@@ -17860,53 +17858,27 @@
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="B278" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="C278" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D278" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="E278" t="s">
         <v>832</v>
       </c>
       <c r="F278" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="G278">
         <v>2</v>
       </c>
       <c r="H278" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>1687</v>
-      </c>
-      <c r="B279" t="s">
-        <v>1688</v>
-      </c>
-      <c r="C279" t="s">
-        <v>1689</v>
-      </c>
-      <c r="D279" t="s">
-        <v>1668</v>
-      </c>
-      <c r="E279" t="s">
-        <v>832</v>
-      </c>
-      <c r="F279" t="s">
-        <v>1688</v>
-      </c>
-      <c r="G279">
-        <v>2</v>
-      </c>
-      <c r="H279" t="s">
         <v>833</v>
       </c>
     </row>

</xml_diff>